<commit_message>
Made PSA flexible in aqueous pages
</commit_message>
<xml_diff>
--- a/Supplementary Workbook Non-Aq.xlsx
+++ b/Supplementary Workbook Non-Aq.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="2603" documentId="8_{31750E0B-A732-4503-8EA8-2753BAB2D178}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DF1D7921-2630-4735-8C67-AF6E9FEF9493}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11295" xr2:uid="{A43CA30C-0C57-4CA9-B7DA-D833452F41BC}"/>
+    <workbookView xWindow="3855" yWindow="3855" windowWidth="21600" windowHeight="11235" xr2:uid="{A43CA30C-0C57-4CA9-B7DA-D833452F41BC}"/>
   </bookViews>
   <sheets>
     <sheet name="Constants and assumptions" sheetId="2" r:id="rId1"/>
@@ -2679,18 +2679,6 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -2712,13 +2700,25 @@
     <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -7707,7 +7707,7 @@
   <dimension ref="A1:F52"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -9443,62 +9443,62 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B1" s="82" t="s">
+      <c r="B1" s="78" t="s">
         <v>226</v>
       </c>
-      <c r="C1" s="82"/>
-      <c r="D1" s="82"/>
-      <c r="E1" s="82"/>
-      <c r="F1" s="82"/>
-      <c r="G1" s="82"/>
-      <c r="H1" s="82"/>
+      <c r="C1" s="78"/>
+      <c r="D1" s="78"/>
+      <c r="E1" s="78"/>
+      <c r="F1" s="78"/>
+      <c r="G1" s="78"/>
+      <c r="H1" s="78"/>
       <c r="I1" s="52"/>
       <c r="J1" s="52"/>
       <c r="K1" s="52"/>
       <c r="S1" s="53"/>
     </row>
     <row r="2" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B2" s="81" t="s">
+      <c r="B2" s="77" t="s">
         <v>225</v>
       </c>
-      <c r="C2" s="81"/>
-      <c r="D2" s="81"/>
-      <c r="E2" s="81"/>
-      <c r="F2" s="81"/>
-      <c r="G2" s="81"/>
-      <c r="H2" s="81"/>
+      <c r="C2" s="77"/>
+      <c r="D2" s="77"/>
+      <c r="E2" s="77"/>
+      <c r="F2" s="77"/>
+      <c r="G2" s="77"/>
+      <c r="H2" s="77"/>
       <c r="I2" s="3"/>
       <c r="J2" s="3"/>
       <c r="K2" s="3"/>
     </row>
     <row r="3" spans="2:19" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="83" t="s">
+      <c r="B3" s="79" t="s">
         <v>227</v>
       </c>
-      <c r="C3" s="83"/>
-      <c r="D3" s="83"/>
-      <c r="E3" s="83"/>
-      <c r="F3" s="83"/>
-      <c r="G3" s="83"/>
-      <c r="H3" s="83"/>
+      <c r="C3" s="79"/>
+      <c r="D3" s="79"/>
+      <c r="E3" s="79"/>
+      <c r="F3" s="79"/>
+      <c r="G3" s="79"/>
+      <c r="H3" s="79"/>
       <c r="I3" s="54"/>
       <c r="J3" s="54"/>
       <c r="K3" s="54"/>
     </row>
     <row r="5" spans="2:19" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="78" t="s">
+      <c r="B5" s="86" t="s">
         <v>224</v>
       </c>
-      <c r="C5" s="78"/>
-      <c r="D5" s="78"/>
-      <c r="E5" s="78"/>
-      <c r="F5" s="78"/>
-      <c r="H5" s="78" t="s">
+      <c r="C5" s="86"/>
+      <c r="D5" s="86"/>
+      <c r="E5" s="86"/>
+      <c r="F5" s="86"/>
+      <c r="H5" s="86" t="s">
         <v>223</v>
       </c>
-      <c r="I5" s="78"/>
-      <c r="J5" s="78"/>
-      <c r="K5" s="78"/>
+      <c r="I5" s="86"/>
+      <c r="J5" s="86"/>
+      <c r="K5" s="86"/>
     </row>
     <row r="6" spans="2:19" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="55"/>
@@ -9736,12 +9736,12 @@
         <f>AVERAGE(K7:K8,K10)</f>
         <v>0.27421105687523872</v>
       </c>
-      <c r="M14" s="87" t="s">
+      <c r="M14" s="83" t="s">
         <v>232</v>
       </c>
-      <c r="N14" s="87"/>
-      <c r="O14" s="87"/>
-      <c r="P14" s="87"/>
+      <c r="N14" s="83"/>
+      <c r="O14" s="83"/>
+      <c r="P14" s="83"/>
     </row>
     <row r="15" spans="2:19" ht="31.5" x14ac:dyDescent="0.25">
       <c r="H15" s="64" t="s">
@@ -9759,10 +9759,10 @@
         <f>STDEV(K7:K8,K10)</f>
         <v>9.5933620789558907E-4</v>
       </c>
-      <c r="M15" s="87"/>
-      <c r="N15" s="87"/>
-      <c r="O15" s="87"/>
-      <c r="P15" s="87"/>
+      <c r="M15" s="83"/>
+      <c r="N15" s="83"/>
+      <c r="O15" s="83"/>
+      <c r="P15" s="83"/>
     </row>
     <row r="16" spans="2:19" ht="31.5" x14ac:dyDescent="0.25">
       <c r="H16" s="64" t="s">
@@ -9783,31 +9783,31 @@
       <c r="M16" s="51"/>
     </row>
     <row r="18" spans="3:21" x14ac:dyDescent="0.25">
-      <c r="C18" s="80" t="s">
+      <c r="C18" s="84" t="s">
         <v>228</v>
       </c>
-      <c r="D18" s="80"/>
-      <c r="E18" s="80"/>
-      <c r="F18" s="80"/>
-      <c r="H18" s="80" t="s">
+      <c r="D18" s="84"/>
+      <c r="E18" s="84"/>
+      <c r="F18" s="84"/>
+      <c r="H18" s="84" t="s">
         <v>229</v>
       </c>
-      <c r="I18" s="80"/>
-      <c r="J18" s="80"/>
-      <c r="K18" s="80"/>
-      <c r="M18" s="80" t="s">
+      <c r="I18" s="84"/>
+      <c r="J18" s="84"/>
+      <c r="K18" s="84"/>
+      <c r="M18" s="84" t="s">
         <v>230</v>
       </c>
-      <c r="N18" s="80"/>
-      <c r="O18" s="80"/>
-      <c r="P18" s="80"/>
+      <c r="N18" s="84"/>
+      <c r="O18" s="84"/>
+      <c r="P18" s="84"/>
       <c r="Q18" s="60"/>
-      <c r="R18" s="80" t="s">
+      <c r="R18" s="84" t="s">
         <v>181</v>
       </c>
-      <c r="S18" s="80"/>
-      <c r="T18" s="80"/>
-      <c r="U18" s="80"/>
+      <c r="S18" s="84"/>
+      <c r="T18" s="84"/>
+      <c r="U18" s="84"/>
     </row>
     <row r="19" spans="3:21" x14ac:dyDescent="0.25">
       <c r="D19" s="60"/>
@@ -9828,7 +9828,7 @@
       <c r="U19" s="60"/>
     </row>
     <row r="20" spans="3:21" ht="44.25" x14ac:dyDescent="0.25">
-      <c r="C20" s="79" t="s">
+      <c r="C20" s="85" t="s">
         <v>208</v>
       </c>
       <c r="D20" s="66"/>
@@ -9838,7 +9838,7 @@
       <c r="F20" s="66" t="s">
         <v>236</v>
       </c>
-      <c r="H20" s="79" t="s">
+      <c r="H20" s="85" t="s">
         <v>208</v>
       </c>
       <c r="I20" s="66"/>
@@ -9848,7 +9848,7 @@
       <c r="K20" s="66" t="s">
         <v>236</v>
       </c>
-      <c r="M20" s="79" t="s">
+      <c r="M20" s="85" t="s">
         <v>208</v>
       </c>
       <c r="N20" s="66"/>
@@ -9859,7 +9859,7 @@
         <v>236</v>
       </c>
       <c r="Q20" s="60"/>
-      <c r="R20" s="79" t="s">
+      <c r="R20" s="85" t="s">
         <v>208</v>
       </c>
       <c r="S20" s="66"/>
@@ -9871,7 +9871,7 @@
       </c>
     </row>
     <row r="21" spans="3:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C21" s="79"/>
+      <c r="C21" s="85"/>
       <c r="D21" s="66" t="s">
         <v>237</v>
       </c>
@@ -9882,7 +9882,7 @@
         <f>$E$75*E23+$F$75</f>
         <v>143.97423691447224</v>
       </c>
-      <c r="H21" s="79"/>
+      <c r="H21" s="85"/>
       <c r="I21" s="66" t="s">
         <v>238</v>
       </c>
@@ -9893,7 +9893,7 @@
         <f>$E$75*J23+$F$75</f>
         <v>161.42236098999606</v>
       </c>
-      <c r="M21" s="79"/>
+      <c r="M21" s="85"/>
       <c r="N21" s="66" t="s">
         <v>237</v>
       </c>
@@ -9905,7 +9905,7 @@
         <v>82.37998906382218</v>
       </c>
       <c r="Q21" s="60"/>
-      <c r="R21" s="79"/>
+      <c r="R21" s="85"/>
       <c r="S21" s="66" t="s">
         <v>238</v>
       </c>
@@ -9918,7 +9918,7 @@
       </c>
     </row>
     <row r="22" spans="3:21" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="C22" s="79"/>
+      <c r="C22" s="85"/>
       <c r="D22" s="66" t="s">
         <v>239</v>
       </c>
@@ -9926,7 +9926,7 @@
         <v>103.6</v>
       </c>
       <c r="F22" s="66"/>
-      <c r="H22" s="79"/>
+      <c r="H22" s="85"/>
       <c r="I22" s="66" t="s">
         <v>239</v>
       </c>
@@ -9934,7 +9934,7 @@
         <v>103.6</v>
       </c>
       <c r="K22" s="67"/>
-      <c r="M22" s="79"/>
+      <c r="M22" s="85"/>
       <c r="N22" s="66" t="s">
         <v>240</v>
       </c>
@@ -9943,7 +9943,7 @@
       </c>
       <c r="P22" s="66"/>
       <c r="Q22" s="60"/>
-      <c r="R22" s="79"/>
+      <c r="R22" s="85"/>
       <c r="S22" s="66" t="s">
         <v>241</v>
       </c>
@@ -9953,7 +9953,7 @@
       <c r="U22" s="66"/>
     </row>
     <row r="23" spans="3:21" x14ac:dyDescent="0.25">
-      <c r="C23" s="79"/>
+      <c r="C23" s="85"/>
       <c r="D23" s="66" t="s">
         <v>216</v>
       </c>
@@ -9962,7 +9962,7 @@
         <v>165.23</v>
       </c>
       <c r="F23" s="66"/>
-      <c r="H23" s="79"/>
+      <c r="H23" s="85"/>
       <c r="I23" s="66" t="s">
         <v>216</v>
       </c>
@@ -9971,7 +9971,7 @@
         <v>188.79</v>
       </c>
       <c r="K23" s="67"/>
-      <c r="M23" s="79"/>
+      <c r="M23" s="85"/>
       <c r="N23" s="66" t="s">
         <v>216</v>
       </c>
@@ -9981,7 +9981,7 @@
       </c>
       <c r="P23" s="66"/>
       <c r="Q23" s="60"/>
-      <c r="R23" s="79"/>
+      <c r="R23" s="85"/>
       <c r="S23" s="66" t="s">
         <v>216</v>
       </c>
@@ -9992,7 +9992,7 @@
       <c r="U23" s="66"/>
     </row>
     <row r="24" spans="3:21" ht="42.75" x14ac:dyDescent="0.25">
-      <c r="C24" s="79"/>
+      <c r="C24" s="85"/>
       <c r="D24" s="65" t="s">
         <v>215</v>
       </c>
@@ -10002,7 +10002,7 @@
       <c r="F24" s="65" t="s">
         <v>213</v>
       </c>
-      <c r="H24" s="79"/>
+      <c r="H24" s="85"/>
       <c r="I24" s="65" t="s">
         <v>215</v>
       </c>
@@ -10012,7 +10012,7 @@
       <c r="K24" s="65" t="s">
         <v>213</v>
       </c>
-      <c r="M24" s="79"/>
+      <c r="M24" s="85"/>
       <c r="N24" s="65" t="s">
         <v>215</v>
       </c>
@@ -10023,7 +10023,7 @@
         <v>213</v>
       </c>
       <c r="Q24" s="60"/>
-      <c r="R24" s="79"/>
+      <c r="R24" s="85"/>
       <c r="S24" s="65" t="s">
         <v>215</v>
       </c>
@@ -10035,7 +10035,7 @@
       </c>
     </row>
     <row r="25" spans="3:21" x14ac:dyDescent="0.25">
-      <c r="C25" s="79"/>
+      <c r="C25" s="85"/>
       <c r="D25" s="68">
         <v>1E-3</v>
       </c>
@@ -10047,7 +10047,7 @@
         <f t="shared" ref="F25:F31" si="1">E25*D25/1000</f>
         <v>1.6067713486965575E-4</v>
       </c>
-      <c r="H25" s="79"/>
+      <c r="H25" s="85"/>
       <c r="I25" s="68">
         <v>1E-3</v>
       </c>
@@ -10059,7 +10059,7 @@
         <f t="shared" ref="K25:K31" si="3">J25*I25/1000</f>
         <v>1.8368537673989698E-4</v>
       </c>
-      <c r="M25" s="79"/>
+      <c r="M25" s="85"/>
       <c r="N25" s="68">
         <v>1E-3</v>
       </c>
@@ -10071,7 +10071,7 @@
         <f t="shared" ref="P25:P31" si="5">O25*N25/1000</f>
         <v>7.94549160093856E-5</v>
       </c>
-      <c r="R25" s="79"/>
+      <c r="R25" s="85"/>
       <c r="S25" s="68">
         <v>1E-3</v>
       </c>
@@ -10085,7 +10085,7 @@
       </c>
     </row>
     <row r="26" spans="3:21" x14ac:dyDescent="0.25">
-      <c r="C26" s="79"/>
+      <c r="C26" s="85"/>
       <c r="D26" s="68">
         <v>2E-3</v>
       </c>
@@ -10097,7 +10097,7 @@
         <f t="shared" si="1"/>
         <v>3.1758255277002323E-4</v>
       </c>
-      <c r="H26" s="79"/>
+      <c r="H26" s="85"/>
       <c r="I26" s="68">
         <v>2E-3</v>
       </c>
@@ -10109,7 +10109,7 @@
         <f t="shared" si="3"/>
         <v>3.6314194510951429E-4</v>
       </c>
-      <c r="M26" s="79"/>
+      <c r="M26" s="85"/>
       <c r="N26" s="68">
         <v>2E-3</v>
       </c>
@@ -10121,7 +10121,7 @@
         <f t="shared" si="5"/>
         <v>1.5675170977870419E-4</v>
       </c>
-      <c r="R26" s="79"/>
+      <c r="R26" s="85"/>
       <c r="S26" s="68">
         <v>2E-3</v>
       </c>
@@ -10135,7 +10135,7 @@
       </c>
     </row>
     <row r="27" spans="3:21" x14ac:dyDescent="0.25">
-      <c r="C27" s="79"/>
+      <c r="C27" s="85"/>
       <c r="D27" s="68">
         <v>3.0000000000000001E-3</v>
       </c>
@@ -10147,7 +10147,7 @@
         <f t="shared" si="1"/>
         <v>4.720326188227051E-4</v>
       </c>
-      <c r="H27" s="79"/>
+      <c r="H27" s="85"/>
       <c r="I27" s="68">
         <v>3.0000000000000001E-3</v>
       </c>
@@ -10159,7 +10159,7 @@
         <f t="shared" si="3"/>
         <v>5.3984559948001105E-4</v>
       </c>
-      <c r="M27" s="79"/>
+      <c r="M27" s="85"/>
       <c r="N27" s="68">
         <v>3.0000000000000001E-3</v>
       </c>
@@ -10171,7 +10171,7 @@
         <f t="shared" si="5"/>
         <v>2.326435865108147E-4</v>
       </c>
-      <c r="R27" s="79"/>
+      <c r="R27" s="85"/>
       <c r="S27" s="68">
         <v>3.0000000000000001E-3</v>
       </c>
@@ -10185,7 +10185,7 @@
       </c>
     </row>
     <row r="28" spans="3:21" x14ac:dyDescent="0.25">
-      <c r="C28" s="79"/>
+      <c r="C28" s="85"/>
       <c r="D28" s="68">
         <v>4.0000000000000001E-3</v>
       </c>
@@ -10197,7 +10197,7 @@
         <f t="shared" si="1"/>
         <v>6.2449707895724602E-4</v>
       </c>
-      <c r="H28" s="79"/>
+      <c r="H28" s="85"/>
       <c r="I28" s="68">
         <v>4.0000000000000001E-3</v>
       </c>
@@ -10209,7 +10209,7 @@
         <f t="shared" si="3"/>
         <v>7.1432301391917592E-4</v>
       </c>
-      <c r="M28" s="79"/>
+      <c r="M28" s="85"/>
       <c r="N28" s="68">
         <v>4.0000000000000001E-3</v>
       </c>
@@ -10221,7 +10221,7 @@
         <f t="shared" si="5"/>
         <v>3.0739932807508481E-4</v>
       </c>
-      <c r="R28" s="79"/>
+      <c r="R28" s="85"/>
       <c r="S28" s="68">
         <v>4.0000000000000001E-3</v>
       </c>
@@ -10235,7 +10235,7 @@
       </c>
     </row>
     <row r="29" spans="3:21" x14ac:dyDescent="0.25">
-      <c r="C29" s="79"/>
+      <c r="C29" s="85"/>
       <c r="D29" s="68">
         <v>0.3</v>
       </c>
@@ -10247,7 +10247,7 @@
         <f t="shared" si="1"/>
         <v>2.5911618822705169E-2</v>
       </c>
-      <c r="H29" s="79"/>
+      <c r="H29" s="85"/>
       <c r="I29" s="68">
         <v>0.3</v>
       </c>
@@ -10259,7 +10259,7 @@
         <f t="shared" si="3"/>
         <v>3.011259948001116E-2</v>
       </c>
-      <c r="M29" s="79"/>
+      <c r="M29" s="85"/>
       <c r="N29" s="68">
         <v>0.3</v>
       </c>
@@ -10271,7 +10271,7 @@
         <f t="shared" si="5"/>
         <v>1.1081586510814711E-2</v>
       </c>
-      <c r="R29" s="79"/>
+      <c r="R29" s="85"/>
       <c r="S29" s="68">
         <v>0.3</v>
       </c>
@@ -10285,7 +10285,7 @@
       </c>
     </row>
     <row r="30" spans="3:21" x14ac:dyDescent="0.25">
-      <c r="C30" s="79"/>
+      <c r="C30" s="85"/>
       <c r="D30" s="68">
         <v>5.0000000000000001E-3</v>
       </c>
@@ -10297,7 +10297,7 @@
         <f t="shared" si="1"/>
         <v>7.7524742038080911E-4</v>
       </c>
-      <c r="H30" s="79"/>
+      <c r="H30" s="85"/>
       <c r="I30" s="68">
         <v>5.0000000000000001E-3</v>
       </c>
@@ -10309,7 +10309,7 @@
         <f t="shared" si="3"/>
         <v>8.8687857695441557E-4</v>
       </c>
-      <c r="M30" s="79"/>
+      <c r="M30" s="85"/>
       <c r="N30" s="68">
         <v>5.0000000000000001E-3</v>
       </c>
@@ -10321,7 +10321,7 @@
         <f t="shared" si="5"/>
         <v>3.8117427554944889E-4</v>
       </c>
-      <c r="R30" s="79"/>
+      <c r="R30" s="85"/>
       <c r="S30" s="68">
         <v>5.0000000000000001E-3</v>
       </c>
@@ -10335,7 +10335,7 @@
       </c>
     </row>
     <row r="31" spans="3:21" x14ac:dyDescent="0.25">
-      <c r="C31" s="79"/>
+      <c r="C31" s="85"/>
       <c r="D31" s="68">
         <v>6.0000000000000001E-3</v>
       </c>
@@ -10347,7 +10347,7 @@
         <f t="shared" si="1"/>
         <v>9.2446682137767929E-4</v>
       </c>
-      <c r="H31" s="79"/>
+      <c r="H31" s="85"/>
       <c r="I31" s="68">
         <v>6.0000000000000001E-3</v>
       </c>
@@ -10359,7 +10359,7 @@
         <f t="shared" si="3"/>
         <v>1.0577176661016314E-3</v>
       </c>
-      <c r="M31" s="79"/>
+      <c r="M31" s="85"/>
       <c r="N31" s="68">
         <v>6.0000000000000001E-3</v>
       </c>
@@ -10371,7 +10371,7 @@
         <f t="shared" si="5"/>
         <v>4.5407324091540811E-4</v>
       </c>
-      <c r="R31" s="79"/>
+      <c r="R31" s="85"/>
       <c r="S31" s="68">
         <v>6.0000000000000001E-3</v>
       </c>
@@ -10388,7 +10388,7 @@
       <c r="C32" s="28"/>
     </row>
     <row r="33" spans="3:21" ht="44.25" x14ac:dyDescent="0.25">
-      <c r="C33" s="79" t="s">
+      <c r="C33" s="85" t="s">
         <v>207</v>
       </c>
       <c r="D33" s="66"/>
@@ -10398,7 +10398,7 @@
       <c r="F33" s="66" t="s">
         <v>236</v>
       </c>
-      <c r="H33" s="79" t="s">
+      <c r="H33" s="85" t="s">
         <v>207</v>
       </c>
       <c r="I33" s="66"/>
@@ -10408,7 +10408,7 @@
       <c r="K33" s="66" t="s">
         <v>236</v>
       </c>
-      <c r="M33" s="79" t="s">
+      <c r="M33" s="85" t="s">
         <v>207</v>
       </c>
       <c r="N33" s="66"/>
@@ -10418,7 +10418,7 @@
       <c r="P33" s="66" t="s">
         <v>236</v>
       </c>
-      <c r="R33" s="79" t="s">
+      <c r="R33" s="85" t="s">
         <v>207</v>
       </c>
       <c r="S33" s="66"/>
@@ -10430,7 +10430,7 @@
       </c>
     </row>
     <row r="34" spans="3:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C34" s="79"/>
+      <c r="C34" s="85"/>
       <c r="D34" s="66" t="s">
         <v>237</v>
       </c>
@@ -10441,7 +10441,7 @@
         <f>$E$76*E36+$F$76</f>
         <v>10.846365318638243</v>
       </c>
-      <c r="H34" s="79"/>
+      <c r="H34" s="85"/>
       <c r="I34" s="66" t="s">
         <v>238</v>
       </c>
@@ -10452,7 +10452,7 @@
         <f>$E$76*J36+$F$76</f>
         <v>12.125442205751522</v>
       </c>
-      <c r="M34" s="79"/>
+      <c r="M34" s="85"/>
       <c r="N34" s="66" t="s">
         <v>237</v>
       </c>
@@ -10463,7 +10463,7 @@
         <f>$E$76*O36+$F$76</f>
         <v>11.300133071447476</v>
       </c>
-      <c r="R34" s="79"/>
+      <c r="R34" s="85"/>
       <c r="S34" s="66" t="s">
         <v>238</v>
       </c>
@@ -10476,7 +10476,7 @@
       </c>
     </row>
     <row r="35" spans="3:21" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="C35" s="79"/>
+      <c r="C35" s="85"/>
       <c r="D35" s="66" t="s">
         <v>239</v>
       </c>
@@ -10484,7 +10484,7 @@
         <v>18.940000000000001</v>
       </c>
       <c r="F35" s="66"/>
-      <c r="H35" s="79"/>
+      <c r="H35" s="85"/>
       <c r="I35" s="66" t="s">
         <v>239</v>
       </c>
@@ -10492,7 +10492,7 @@
         <v>18.940000000000001</v>
       </c>
       <c r="K35" s="66"/>
-      <c r="M35" s="79"/>
+      <c r="M35" s="85"/>
       <c r="N35" s="66" t="s">
         <v>240</v>
       </c>
@@ -10500,7 +10500,7 @@
         <v>20.43</v>
       </c>
       <c r="P35" s="66"/>
-      <c r="R35" s="79"/>
+      <c r="R35" s="85"/>
       <c r="S35" s="66" t="s">
         <v>241</v>
       </c>
@@ -10510,7 +10510,7 @@
       <c r="U35" s="66"/>
     </row>
     <row r="36" spans="3:21" x14ac:dyDescent="0.25">
-      <c r="C36" s="79"/>
+      <c r="C36" s="85"/>
       <c r="D36" s="66" t="s">
         <v>216</v>
       </c>
@@ -10519,7 +10519,7 @@
         <v>27.92</v>
       </c>
       <c r="F36" s="66"/>
-      <c r="H36" s="79"/>
+      <c r="H36" s="85"/>
       <c r="I36" s="66" t="s">
         <v>216</v>
       </c>
@@ -10528,7 +10528,7 @@
         <v>32.120000000000005</v>
       </c>
       <c r="K36" s="67"/>
-      <c r="M36" s="79"/>
+      <c r="M36" s="85"/>
       <c r="N36" s="66" t="s">
         <v>216</v>
       </c>
@@ -10538,7 +10538,7 @@
       </c>
       <c r="P36" s="66"/>
       <c r="Q36" s="60"/>
-      <c r="R36" s="79"/>
+      <c r="R36" s="85"/>
       <c r="S36" s="66" t="s">
         <v>216</v>
       </c>
@@ -10549,7 +10549,7 @@
       <c r="U36" s="66"/>
     </row>
     <row r="37" spans="3:21" ht="42.75" x14ac:dyDescent="0.25">
-      <c r="C37" s="79"/>
+      <c r="C37" s="85"/>
       <c r="D37" s="65" t="s">
         <v>215</v>
       </c>
@@ -10559,7 +10559,7 @@
       <c r="F37" s="65" t="s">
         <v>213</v>
       </c>
-      <c r="H37" s="79"/>
+      <c r="H37" s="85"/>
       <c r="I37" s="65" t="s">
         <v>215</v>
       </c>
@@ -10569,7 +10569,7 @@
       <c r="K37" s="65" t="s">
         <v>213</v>
       </c>
-      <c r="M37" s="79"/>
+      <c r="M37" s="85"/>
       <c r="N37" s="65" t="s">
         <v>215</v>
       </c>
@@ -10580,7 +10580,7 @@
         <v>213</v>
       </c>
       <c r="Q37" s="60"/>
-      <c r="R37" s="79"/>
+      <c r="R37" s="85"/>
       <c r="S37" s="65" t="s">
         <v>215</v>
       </c>
@@ -10592,7 +10592,7 @@
       </c>
     </row>
     <row r="38" spans="3:21" x14ac:dyDescent="0.25">
-      <c r="C38" s="79"/>
+      <c r="C38" s="85"/>
       <c r="D38" s="68">
         <v>1E-3</v>
       </c>
@@ -10604,7 +10604,7 @@
         <f t="shared" ref="F38:F44" si="9">E38*D38/1000</f>
         <v>2.7577007812588457E-5</v>
       </c>
-      <c r="H38" s="79"/>
+      <c r="H38" s="85"/>
       <c r="I38" s="68">
         <v>1E-3</v>
       </c>
@@ -10616,7 +10616,7 @@
         <f t="shared" ref="K38:K44" si="11">J38*I38/1000</f>
         <v>3.1736559849930896E-5</v>
       </c>
-      <c r="M38" s="79"/>
+      <c r="M38" s="85"/>
       <c r="N38" s="68">
         <v>1E-3</v>
       </c>
@@ -10628,7 +10628,7 @@
         <f t="shared" ref="P38:P44" si="13">O38*N38/1000</f>
         <v>2.9052658416312318E-5</v>
       </c>
-      <c r="R38" s="79"/>
+      <c r="R38" s="85"/>
       <c r="S38" s="68">
         <v>1E-3</v>
       </c>
@@ -10642,7 +10642,7 @@
       </c>
     </row>
     <row r="39" spans="3:21" x14ac:dyDescent="0.25">
-      <c r="C39" s="79"/>
+      <c r="C39" s="85"/>
       <c r="D39" s="68">
         <v>2E-3</v>
       </c>
@@ -10654,7 +10654,7 @@
         <f t="shared" si="9"/>
         <v>5.4869871593549151E-5</v>
       </c>
-      <c r="H39" s="79"/>
+      <c r="H39" s="85"/>
       <c r="I39" s="68">
         <v>2E-3</v>
       </c>
@@ -10666,7 +10666,7 @@
         <f t="shared" si="11"/>
         <v>6.3155467478827784E-5</v>
       </c>
-      <c r="M39" s="79"/>
+      <c r="M39" s="85"/>
       <c r="N39" s="68">
         <v>2E-3</v>
       </c>
@@ -10678,7 +10678,7 @@
         <f t="shared" si="13"/>
         <v>5.7809285371898002E-5</v>
       </c>
-      <c r="R39" s="79"/>
+      <c r="R39" s="85"/>
       <c r="S39" s="68">
         <v>2E-3</v>
       </c>
@@ -10692,7 +10692,7 @@
       </c>
     </row>
     <row r="40" spans="3:21" x14ac:dyDescent="0.25">
-      <c r="C40" s="79"/>
+      <c r="C40" s="85"/>
       <c r="D40" s="68">
         <v>3.0000000000000001E-3</v>
       </c>
@@ -10704,7 +10704,7 @@
         <f t="shared" si="9"/>
         <v>8.1977760314412034E-5</v>
       </c>
-      <c r="H40" s="79"/>
+      <c r="H40" s="85"/>
       <c r="I40" s="68">
         <v>3.0000000000000001E-3</v>
       </c>
@@ -10716,7 +10716,7 @@
         <f t="shared" si="11"/>
         <v>9.4367586535255423E-5</v>
       </c>
-      <c r="M40" s="79"/>
+      <c r="M40" s="85"/>
       <c r="N40" s="68">
         <v>3.0000000000000001E-3</v>
       </c>
@@ -10728,7 +10728,7 @@
         <f t="shared" si="13"/>
         <v>8.6373198664187431E-5</v>
       </c>
-      <c r="R40" s="79"/>
+      <c r="R40" s="85"/>
       <c r="S40" s="68">
         <v>3.0000000000000001E-3</v>
       </c>
@@ -10742,7 +10742,7 @@
       </c>
     </row>
     <row r="41" spans="3:21" x14ac:dyDescent="0.25">
-      <c r="C41" s="79"/>
+      <c r="C41" s="85"/>
       <c r="D41" s="68">
         <v>4.0000000000000001E-3</v>
       </c>
@@ -10754,7 +10754,7 @@
         <f t="shared" si="9"/>
         <v>1.0893606250070763E-4</v>
       </c>
-      <c r="H41" s="79"/>
+      <c r="H41" s="85"/>
       <c r="I41" s="68">
         <v>4.0000000000000001E-3</v>
       </c>
@@ -10766,7 +10766,7 @@
         <f t="shared" si="11"/>
         <v>1.2541247879944718E-4</v>
       </c>
-      <c r="M41" s="79"/>
+      <c r="M41" s="85"/>
       <c r="N41" s="68">
         <v>4.0000000000000001E-3</v>
       </c>
@@ -10778,7 +10778,7 @@
         <f t="shared" si="13"/>
         <v>1.1478126733049854E-4</v>
       </c>
-      <c r="R41" s="79"/>
+      <c r="R41" s="85"/>
       <c r="S41" s="68">
         <v>4.0000000000000001E-3</v>
       </c>
@@ -10792,7 +10792,7 @@
       </c>
     </row>
     <row r="42" spans="3:21" x14ac:dyDescent="0.25">
-      <c r="C42" s="79"/>
+      <c r="C42" s="85"/>
       <c r="D42" s="68">
         <v>0.3</v>
       </c>
@@ -10804,7 +10804,7 @@
         <f t="shared" si="9"/>
         <v>6.5937603144120387E-3</v>
       </c>
-      <c r="H42" s="79"/>
+      <c r="H42" s="85"/>
       <c r="I42" s="68">
         <v>0.3</v>
       </c>
@@ -10816,7 +10816,7 @@
         <f t="shared" si="11"/>
         <v>7.6435865352554094E-3</v>
       </c>
-      <c r="M42" s="79"/>
+      <c r="M42" s="85"/>
       <c r="N42" s="68">
         <v>0.3</v>
       </c>
@@ -10828,7 +10828,7 @@
         <f t="shared" si="13"/>
         <v>6.9661986641874245E-3</v>
       </c>
-      <c r="R42" s="79"/>
+      <c r="R42" s="85"/>
       <c r="S42" s="68">
         <v>0.3</v>
       </c>
@@ -10842,7 +10842,7 @@
       </c>
     </row>
     <row r="43" spans="3:21" x14ac:dyDescent="0.25">
-      <c r="C43" s="79"/>
+      <c r="C43" s="85"/>
       <c r="D43" s="68">
         <v>5.0000000000000001E-3</v>
       </c>
@@ -10854,7 +10854,7 @@
         <f t="shared" si="9"/>
         <v>1.3576523076598215E-4</v>
       </c>
-      <c r="H43" s="79"/>
+      <c r="H43" s="85"/>
       <c r="I43" s="68">
         <v>5.0000000000000001E-3</v>
       </c>
@@ -10866,7 +10866,7 @@
         <f t="shared" si="11"/>
         <v>1.563130087957138E-4</v>
       </c>
-      <c r="M43" s="79"/>
+      <c r="M43" s="85"/>
       <c r="N43" s="68">
         <v>5.0000000000000001E-3</v>
       </c>
@@ -10878,7 +10878,7 @@
         <f t="shared" si="13"/>
         <v>1.4305479963843456E-4</v>
       </c>
-      <c r="R43" s="79"/>
+      <c r="R43" s="85"/>
       <c r="S43" s="68">
         <v>5.0000000000000001E-3</v>
       </c>
@@ -10892,7 +10892,7 @@
       </c>
     </row>
     <row r="44" spans="3:21" x14ac:dyDescent="0.25">
-      <c r="C44" s="79"/>
+      <c r="C44" s="85"/>
       <c r="D44" s="68">
         <v>6.0000000000000001E-3</v>
       </c>
@@ -10904,7 +10904,7 @@
         <f t="shared" si="9"/>
         <v>1.6247906493048388E-4</v>
       </c>
-      <c r="H44" s="79"/>
+      <c r="H44" s="85"/>
       <c r="I44" s="68">
         <v>6.0000000000000001E-3</v>
       </c>
@@ -10916,7 +10916,7 @@
         <f t="shared" si="11"/>
         <v>1.8708460371260688E-4</v>
       </c>
-      <c r="M44" s="79"/>
+      <c r="M44" s="85"/>
       <c r="N44" s="68">
         <v>6.0000000000000001E-3</v>
       </c>
@@ -10928,7 +10928,7 @@
         <f t="shared" si="13"/>
         <v>1.7120817273652276E-4</v>
       </c>
-      <c r="R44" s="79"/>
+      <c r="R44" s="85"/>
       <c r="S44" s="68">
         <v>6.0000000000000001E-3</v>
       </c>
@@ -10945,7 +10945,7 @@
       <c r="C45" s="28"/>
     </row>
     <row r="46" spans="3:21" ht="44.25" x14ac:dyDescent="0.25">
-      <c r="C46" s="79" t="s">
+      <c r="C46" s="85" t="s">
         <v>169</v>
       </c>
       <c r="D46" s="66"/>
@@ -10955,7 +10955,7 @@
       <c r="F46" s="66" t="s">
         <v>236</v>
       </c>
-      <c r="H46" s="79" t="s">
+      <c r="H46" s="85" t="s">
         <v>169</v>
       </c>
       <c r="I46" s="66"/>
@@ -10965,7 +10965,7 @@
       <c r="K46" s="66" t="s">
         <v>236</v>
       </c>
-      <c r="M46" s="79" t="s">
+      <c r="M46" s="85" t="s">
         <v>169</v>
       </c>
       <c r="N46" s="66"/>
@@ -10975,7 +10975,7 @@
       <c r="P46" s="66" t="s">
         <v>236</v>
       </c>
-      <c r="R46" s="79" t="s">
+      <c r="R46" s="85" t="s">
         <v>169</v>
       </c>
       <c r="S46" s="66"/>
@@ -10987,7 +10987,7 @@
       </c>
     </row>
     <row r="47" spans="3:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C47" s="79"/>
+      <c r="C47" s="85"/>
       <c r="D47" s="66" t="s">
         <v>237</v>
       </c>
@@ -10998,7 +10998,7 @@
         <f>$E$77*E49+$F$77</f>
         <v>66.019453701004863</v>
       </c>
-      <c r="H47" s="79"/>
+      <c r="H47" s="85"/>
       <c r="I47" s="66" t="s">
         <v>238</v>
       </c>
@@ -11009,7 +11009,7 @@
         <f>$E$77*J49+$F$77</f>
         <v>72.962336087810144</v>
       </c>
-      <c r="M47" s="79"/>
+      <c r="M47" s="85"/>
       <c r="N47" s="66" t="s">
         <v>237</v>
       </c>
@@ -11020,7 +11020,7 @@
         <f>$E$77*O49+$F$77</f>
         <v>55.938302495395973</v>
       </c>
-      <c r="R47" s="79"/>
+      <c r="R47" s="85"/>
       <c r="S47" s="66" t="s">
         <v>238</v>
       </c>
@@ -11033,7 +11033,7 @@
       </c>
     </row>
     <row r="48" spans="3:21" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="C48" s="79"/>
+      <c r="C48" s="85"/>
       <c r="D48" s="66" t="s">
         <v>239</v>
       </c>
@@ -11041,7 +11041,7 @@
         <v>51.6</v>
       </c>
       <c r="F48" s="66"/>
-      <c r="H48" s="79"/>
+      <c r="H48" s="85"/>
       <c r="I48" s="66" t="s">
         <v>239</v>
       </c>
@@ -11049,7 +11049,7 @@
         <v>51.6</v>
       </c>
       <c r="K48" s="66"/>
-      <c r="M48" s="79"/>
+      <c r="M48" s="85"/>
       <c r="N48" s="66" t="s">
         <v>240</v>
       </c>
@@ -11057,7 +11057,7 @@
         <v>37.53</v>
       </c>
       <c r="P48" s="66"/>
-      <c r="R48" s="79"/>
+      <c r="R48" s="85"/>
       <c r="S48" s="66" t="s">
         <v>241</v>
       </c>
@@ -11067,7 +11067,7 @@
       <c r="U48" s="66"/>
     </row>
     <row r="49" spans="3:21" x14ac:dyDescent="0.25">
-      <c r="C49" s="79"/>
+      <c r="C49" s="85"/>
       <c r="D49" s="66" t="s">
         <v>216</v>
       </c>
@@ -11076,7 +11076,7 @@
         <v>78.28</v>
       </c>
       <c r="F49" s="66"/>
-      <c r="H49" s="79"/>
+      <c r="H49" s="85"/>
       <c r="I49" s="66" t="s">
         <v>216</v>
       </c>
@@ -11085,7 +11085,7 @@
         <v>87.97</v>
       </c>
       <c r="K49" s="67"/>
-      <c r="M49" s="79"/>
+      <c r="M49" s="85"/>
       <c r="N49" s="66" t="s">
         <v>216</v>
       </c>
@@ -11095,7 +11095,7 @@
       </c>
       <c r="P49" s="66"/>
       <c r="Q49" s="60"/>
-      <c r="R49" s="79"/>
+      <c r="R49" s="85"/>
       <c r="S49" s="66" t="s">
         <v>216</v>
       </c>
@@ -11106,7 +11106,7 @@
       <c r="U49" s="66"/>
     </row>
     <row r="50" spans="3:21" ht="42.75" x14ac:dyDescent="0.25">
-      <c r="C50" s="79"/>
+      <c r="C50" s="85"/>
       <c r="D50" s="65" t="s">
         <v>215</v>
       </c>
@@ -11116,7 +11116,7 @@
       <c r="F50" s="65" t="s">
         <v>213</v>
       </c>
-      <c r="H50" s="79"/>
+      <c r="H50" s="85"/>
       <c r="I50" s="65" t="s">
         <v>215</v>
       </c>
@@ -11126,7 +11126,7 @@
       <c r="K50" s="65" t="s">
         <v>213</v>
       </c>
-      <c r="M50" s="79"/>
+      <c r="M50" s="85"/>
       <c r="N50" s="65" t="s">
         <v>215</v>
       </c>
@@ -11137,7 +11137,7 @@
         <v>213</v>
       </c>
       <c r="Q50" s="60"/>
-      <c r="R50" s="79"/>
+      <c r="R50" s="85"/>
       <c r="S50" s="65" t="s">
         <v>215</v>
       </c>
@@ -11149,7 +11149,7 @@
       </c>
     </row>
     <row r="51" spans="3:21" x14ac:dyDescent="0.25">
-      <c r="C51" s="79"/>
+      <c r="C51" s="85"/>
       <c r="D51" s="68">
         <v>1E-3</v>
       </c>
@@ -11161,7 +11161,7 @@
         <f t="shared" ref="F51:F57" si="17">E51*D51/1000</f>
         <v>7.6192281564247928E-5</v>
       </c>
-      <c r="H51" s="79"/>
+      <c r="H51" s="85"/>
       <c r="I51" s="68">
         <v>1E-3</v>
       </c>
@@ -11173,7 +11173,7 @@
         <f t="shared" ref="K51:K57" si="19">J51*I51/1000</f>
         <v>8.5662728345558216E-5</v>
       </c>
-      <c r="M51" s="79"/>
+      <c r="M51" s="85"/>
       <c r="N51" s="68">
         <v>1E-3</v>
       </c>
@@ -11185,7 +11185,7 @@
         <f t="shared" ref="P51:P57" si="21">O51*N51/1000</f>
         <v>6.2441075556710703E-5</v>
       </c>
-      <c r="R51" s="79"/>
+      <c r="R51" s="85"/>
       <c r="S51" s="68">
         <v>1E-3</v>
       </c>
@@ -11199,7 +11199,7 @@
       </c>
     </row>
     <row r="52" spans="3:21" x14ac:dyDescent="0.25">
-      <c r="C52" s="79"/>
+      <c r="C52" s="85"/>
       <c r="D52" s="68">
         <v>2E-3</v>
       </c>
@@ -11211,7 +11211,7 @@
         <f t="shared" si="17"/>
         <v>1.5065504054748613E-4</v>
       </c>
-      <c r="H52" s="79"/>
+      <c r="H52" s="85"/>
       <c r="I52" s="68">
         <v>2E-3</v>
       </c>
@@ -11223,7 +11223,7 @@
         <f t="shared" si="19"/>
         <v>1.694140502684188E-4</v>
       </c>
-      <c r="M52" s="79"/>
+      <c r="M52" s="85"/>
       <c r="N52" s="68">
         <v>2E-3</v>
       </c>
@@ -11235,7 +11235,7 @@
         <f t="shared" si="21"/>
         <v>1.2341672612297395E-4</v>
       </c>
-      <c r="R52" s="79"/>
+      <c r="R52" s="85"/>
       <c r="S52" s="68">
         <v>2E-3</v>
       </c>
@@ -11249,7 +11249,7 @@
       </c>
     </row>
     <row r="53" spans="3:21" x14ac:dyDescent="0.25">
-      <c r="C53" s="79"/>
+      <c r="C53" s="85"/>
       <c r="D53" s="68">
         <v>3.0000000000000001E-3</v>
       </c>
@@ -11261,7 +11261,7 @@
         <f t="shared" si="17"/>
         <v>2.2399189679213753E-4</v>
       </c>
-      <c r="H53" s="79"/>
+      <c r="H53" s="85"/>
       <c r="I53" s="68">
         <v>3.0000000000000001E-3</v>
       </c>
@@ -11273,7 +11273,7 @@
         <f t="shared" si="19"/>
         <v>2.519210648029299E-4</v>
       </c>
-      <c r="M53" s="79"/>
+      <c r="M53" s="85"/>
       <c r="N53" s="68">
         <v>3.0000000000000001E-3</v>
       </c>
@@ -11285,7 +11285,7 @@
         <f t="shared" si="21"/>
         <v>1.8343839896841726E-4</v>
       </c>
-      <c r="R53" s="79"/>
+      <c r="R53" s="85"/>
       <c r="S53" s="68">
         <v>3.0000000000000001E-3</v>
       </c>
@@ -11299,7 +11299,7 @@
       </c>
     </row>
     <row r="54" spans="3:21" x14ac:dyDescent="0.25">
-      <c r="C54" s="79"/>
+      <c r="C54" s="85"/>
       <c r="D54" s="68">
         <v>4.0000000000000001E-3</v>
       </c>
@@ -11311,7 +11311,7 @@
         <f t="shared" si="17"/>
         <v>2.9641825251398336E-4</v>
       </c>
-      <c r="H54" s="79"/>
+      <c r="H54" s="85"/>
       <c r="I54" s="68">
         <v>4.0000000000000001E-3</v>
       </c>
@@ -11323,7 +11323,7 @@
         <f t="shared" si="19"/>
         <v>3.3342182676446568E-4</v>
       </c>
-      <c r="M54" s="79"/>
+      <c r="M54" s="85"/>
       <c r="N54" s="68">
         <v>4.0000000000000001E-3</v>
       </c>
@@ -11335,7 +11335,7 @@
         <f t="shared" si="21"/>
         <v>2.4268860445368547E-4</v>
       </c>
-      <c r="R54" s="79"/>
+      <c r="R54" s="85"/>
       <c r="S54" s="68">
         <v>4.0000000000000001E-3</v>
       </c>
@@ -11349,7 +11349,7 @@
       </c>
     </row>
     <row r="55" spans="3:21" x14ac:dyDescent="0.25">
-      <c r="C55" s="79"/>
+      <c r="C55" s="85"/>
       <c r="D55" s="68">
         <v>0.3</v>
       </c>
@@ -11361,7 +11361,7 @@
         <f t="shared" si="17"/>
         <v>1.2635896792137514E-2</v>
       </c>
-      <c r="H55" s="79"/>
+      <c r="H55" s="85"/>
       <c r="I55" s="68">
         <v>0.3</v>
       </c>
@@ -11373,7 +11373,7 @@
         <f t="shared" si="19"/>
         <v>1.4402064802929944E-2</v>
       </c>
-      <c r="M55" s="79"/>
+      <c r="M55" s="85"/>
       <c r="N55" s="68">
         <v>0.3</v>
       </c>
@@ -11385,7 +11385,7 @@
         <f t="shared" si="21"/>
         <v>1.0071398968417234E-2</v>
       </c>
-      <c r="R55" s="79"/>
+      <c r="R55" s="85"/>
       <c r="S55" s="68">
         <v>0.3</v>
       </c>
@@ -11399,7 +11399,7 @@
       </c>
     </row>
     <row r="56" spans="3:21" x14ac:dyDescent="0.25">
-      <c r="C56" s="79"/>
+      <c r="C56" s="85"/>
       <c r="D56" s="68">
         <v>5.0000000000000001E-3</v>
       </c>
@@ -11411,7 +11411,7 @@
         <f t="shared" si="17"/>
         <v>3.6805859829889409E-4</v>
       </c>
-      <c r="H56" s="79"/>
+      <c r="H56" s="85"/>
       <c r="I56" s="68">
         <v>5.0000000000000001E-3</v>
       </c>
@@ -11423,7 +11423,7 @@
         <f t="shared" si="19"/>
         <v>4.1405391869054877E-4</v>
       </c>
-      <c r="M56" s="79"/>
+      <c r="M56" s="85"/>
       <c r="N56" s="68">
         <v>5.0000000000000001E-3</v>
       </c>
@@ -11435,7 +11435,7 @@
         <f t="shared" si="21"/>
         <v>3.0127282348872063E-4</v>
       </c>
-      <c r="R56" s="79"/>
+      <c r="R56" s="85"/>
       <c r="S56" s="68">
         <v>5.0000000000000001E-3</v>
       </c>
@@ -11449,7 +11449,7 @@
       </c>
     </row>
     <row r="57" spans="3:21" x14ac:dyDescent="0.25">
-      <c r="C57" s="79"/>
+      <c r="C57" s="85"/>
       <c r="D57" s="68">
         <v>6.0000000000000001E-3</v>
       </c>
@@ -11461,7 +11461,7 @@
         <f t="shared" si="17"/>
         <v>4.3899693063483556E-4</v>
       </c>
-      <c r="H57" s="79"/>
+      <c r="H57" s="85"/>
       <c r="I57" s="68">
         <v>6.0000000000000001E-3</v>
       </c>
@@ -11473,7 +11473,7 @@
         <f t="shared" si="19"/>
         <v>4.9391017049178266E-4</v>
       </c>
-      <c r="M57" s="79"/>
+      <c r="M57" s="85"/>
       <c r="N57" s="68">
         <v>6.0000000000000001E-3</v>
       </c>
@@ -11485,7 +11485,7 @@
         <f t="shared" si="21"/>
         <v>3.5926222632242624E-4</v>
       </c>
-      <c r="R57" s="79"/>
+      <c r="R57" s="85"/>
       <c r="S57" s="68">
         <v>6.0000000000000001E-3</v>
       </c>
@@ -11502,7 +11502,7 @@
       <c r="C58" s="28"/>
     </row>
     <row r="59" spans="3:21" ht="44.25" x14ac:dyDescent="0.25">
-      <c r="C59" s="79" t="s">
+      <c r="C59" s="85" t="s">
         <v>154</v>
       </c>
       <c r="D59" s="66"/>
@@ -11512,7 +11512,7 @@
       <c r="F59" s="66" t="s">
         <v>236</v>
       </c>
-      <c r="H59" s="79" t="s">
+      <c r="H59" s="85" t="s">
         <v>154</v>
       </c>
       <c r="I59" s="66"/>
@@ -11522,7 +11522,7 @@
       <c r="K59" s="66" t="s">
         <v>236</v>
       </c>
-      <c r="M59" s="84" t="s">
+      <c r="M59" s="80" t="s">
         <v>154</v>
       </c>
       <c r="N59" s="66"/>
@@ -11532,7 +11532,7 @@
       <c r="P59" s="66" t="s">
         <v>236</v>
       </c>
-      <c r="R59" s="79" t="s">
+      <c r="R59" s="85" t="s">
         <v>154</v>
       </c>
       <c r="S59" s="66"/>
@@ -11544,7 +11544,7 @@
       </c>
     </row>
     <row r="60" spans="3:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C60" s="79"/>
+      <c r="C60" s="85"/>
       <c r="D60" s="66" t="s">
         <v>237</v>
       </c>
@@ -11555,7 +11555,7 @@
         <f>$E$78*E62+$F$78</f>
         <v>21.270014007783026</v>
       </c>
-      <c r="H60" s="79"/>
+      <c r="H60" s="85"/>
       <c r="I60" s="66" t="s">
         <v>238</v>
       </c>
@@ -11566,7 +11566,7 @@
         <f>$E$78*J62+$F$78</f>
         <v>24.013030008855846</v>
       </c>
-      <c r="M60" s="85"/>
+      <c r="M60" s="81"/>
       <c r="N60" s="66" t="s">
         <v>237</v>
       </c>
@@ -11577,7 +11577,7 @@
         <f>$E$78*O62+$F$78</f>
         <v>22.39033006682925</v>
       </c>
-      <c r="R60" s="79"/>
+      <c r="R60" s="85"/>
       <c r="S60" s="66" t="s">
         <v>238</v>
       </c>
@@ -11590,7 +11590,7 @@
       </c>
     </row>
     <row r="61" spans="3:21" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="C61" s="79"/>
+      <c r="C61" s="85"/>
       <c r="D61" s="66" t="s">
         <v>239</v>
       </c>
@@ -11598,7 +11598,7 @@
         <v>24.39</v>
       </c>
       <c r="F61" s="66"/>
-      <c r="H61" s="79"/>
+      <c r="H61" s="85"/>
       <c r="I61" s="66" t="s">
         <v>239</v>
       </c>
@@ -11606,7 +11606,7 @@
         <v>24.39</v>
       </c>
       <c r="K61" s="66"/>
-      <c r="M61" s="85"/>
+      <c r="M61" s="81"/>
       <c r="N61" s="66" t="s">
         <v>240</v>
       </c>
@@ -11614,7 +11614,7 @@
         <v>26.62</v>
       </c>
       <c r="P61" s="66"/>
-      <c r="R61" s="79"/>
+      <c r="R61" s="85"/>
       <c r="S61" s="66" t="s">
         <v>241</v>
       </c>
@@ -11624,7 +11624,7 @@
       <c r="U61" s="66"/>
     </row>
     <row r="62" spans="3:21" x14ac:dyDescent="0.25">
-      <c r="C62" s="79"/>
+      <c r="C62" s="85"/>
       <c r="D62" s="66" t="s">
         <v>216</v>
       </c>
@@ -11633,7 +11633,7 @@
         <v>35.32</v>
       </c>
       <c r="F62" s="66"/>
-      <c r="H62" s="79"/>
+      <c r="H62" s="85"/>
       <c r="I62" s="66" t="s">
         <v>216</v>
       </c>
@@ -11642,7 +11642,7 @@
         <v>40.78</v>
       </c>
       <c r="K62" s="67"/>
-      <c r="M62" s="85"/>
+      <c r="M62" s="81"/>
       <c r="N62" s="66" t="s">
         <v>216</v>
       </c>
@@ -11652,7 +11652,7 @@
       </c>
       <c r="P62" s="66"/>
       <c r="Q62" s="60"/>
-      <c r="R62" s="79"/>
+      <c r="R62" s="85"/>
       <c r="S62" s="66" t="s">
         <v>216</v>
       </c>
@@ -11663,7 +11663,7 @@
       <c r="U62" s="66"/>
     </row>
     <row r="63" spans="3:21" ht="42.75" x14ac:dyDescent="0.25">
-      <c r="C63" s="79"/>
+      <c r="C63" s="85"/>
       <c r="D63" s="65" t="s">
         <v>215</v>
       </c>
@@ -11673,7 +11673,7 @@
       <c r="F63" s="65" t="s">
         <v>213</v>
       </c>
-      <c r="H63" s="79"/>
+      <c r="H63" s="85"/>
       <c r="I63" s="65" t="s">
         <v>215</v>
       </c>
@@ -11683,7 +11683,7 @@
       <c r="K63" s="65" t="s">
         <v>213</v>
       </c>
-      <c r="M63" s="85"/>
+      <c r="M63" s="81"/>
       <c r="N63" s="65" t="s">
         <v>215</v>
       </c>
@@ -11694,7 +11694,7 @@
         <v>213</v>
       </c>
       <c r="Q63" s="60"/>
-      <c r="R63" s="79"/>
+      <c r="R63" s="85"/>
       <c r="S63" s="65" t="s">
         <v>215</v>
       </c>
@@ -11706,7 +11706,7 @@
       </c>
     </row>
     <row r="64" spans="3:21" x14ac:dyDescent="0.25">
-      <c r="C64" s="79"/>
+      <c r="C64" s="85"/>
       <c r="D64" s="68">
         <v>1E-3</v>
       </c>
@@ -11718,7 +11718,7 @@
         <f t="shared" ref="F64:F70" si="25">E64*D64/1000</f>
         <v>3.4647383098717194E-5</v>
       </c>
-      <c r="H64" s="79"/>
+      <c r="H64" s="85"/>
       <c r="I64" s="68">
         <v>1E-3</v>
       </c>
@@ -11730,7 +11730,7 @@
         <f t="shared" ref="K64:K70" si="27">J64*I64/1000</f>
         <v>4.0020641316500427E-5</v>
       </c>
-      <c r="M64" s="85"/>
+      <c r="M64" s="81"/>
       <c r="N64" s="68">
         <v>1E-3</v>
       </c>
@@ -11742,7 +11742,7 @@
         <f t="shared" ref="P64:P70" si="29">O64*N64/1000</f>
         <v>3.6841955594258693E-5</v>
       </c>
-      <c r="R64" s="79"/>
+      <c r="R64" s="85"/>
       <c r="S64" s="68">
         <v>1E-3</v>
       </c>
@@ -11756,7 +11756,7 @@
       </c>
     </row>
     <row r="65" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="C65" s="79"/>
+      <c r="C65" s="85"/>
       <c r="D65" s="68">
         <v>2E-3</v>
       </c>
@@ -11768,7 +11768,7 @@
         <f t="shared" si="25"/>
         <v>6.8737552111848972E-5</v>
       </c>
-      <c r="H65" s="79"/>
+      <c r="H65" s="85"/>
       <c r="I65" s="68">
         <v>2E-3</v>
       </c>
@@ -11780,7 +11780,7 @@
         <f t="shared" si="27"/>
         <v>7.9412209302178241E-5</v>
       </c>
-      <c r="M65" s="85"/>
+      <c r="M65" s="81"/>
       <c r="N65" s="68">
         <v>2E-3</v>
       </c>
@@ -11792,7 +11792,7 @@
         <f t="shared" si="29"/>
         <v>7.3097347997276484E-5</v>
       </c>
-      <c r="R65" s="79"/>
+      <c r="R65" s="85"/>
       <c r="S65" s="68">
         <v>2E-3</v>
       </c>
@@ -11806,7 +11806,7 @@
       </c>
     </row>
     <row r="66" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="C66" s="79"/>
+      <c r="C66" s="85"/>
       <c r="D66" s="68">
         <v>3.0000000000000001E-3</v>
       </c>
@@ -11818,7 +11818,7 @@
         <f t="shared" si="25"/>
         <v>1.0246498005884591E-4</v>
       </c>
-      <c r="H66" s="79"/>
+      <c r="H66" s="85"/>
       <c r="I66" s="68">
         <v>3.0000000000000001E-3</v>
       </c>
@@ -11830,7 +11830,7 @@
         <f t="shared" si="27"/>
         <v>1.1839425653703035E-4</v>
       </c>
-      <c r="M66" s="85"/>
+      <c r="M66" s="81"/>
       <c r="N66" s="68">
         <v>3.0000000000000001E-3</v>
       </c>
@@ -11842,7 +11842,7 @@
         <f t="shared" si="29"/>
         <v>1.0897089334572343E-4</v>
       </c>
-      <c r="R66" s="79"/>
+      <c r="R66" s="85"/>
       <c r="S66" s="68">
         <v>3.0000000000000001E-3</v>
       </c>
@@ -11856,7 +11856,7 @@
       </c>
     </row>
     <row r="67" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="C67" s="79"/>
+      <c r="C67" s="85"/>
       <c r="D67" s="68">
         <v>4.0000000000000001E-3</v>
       </c>
@@ -11868,7 +11868,7 @@
         <f t="shared" si="25"/>
         <v>1.3589906478973755E-4</v>
       </c>
-      <c r="H67" s="79"/>
+      <c r="H67" s="85"/>
       <c r="I67" s="68">
         <v>4.0000000000000001E-3</v>
       </c>
@@ -11880,7 +11880,7 @@
         <f t="shared" si="27"/>
         <v>1.5704513053200339E-4</v>
       </c>
-      <c r="M67" s="85"/>
+      <c r="M67" s="81"/>
       <c r="N67" s="68">
         <v>4.0000000000000001E-3</v>
       </c>
@@ -11892,7 +11892,7 @@
         <f t="shared" si="29"/>
         <v>1.4453564475406955E-4</v>
       </c>
-      <c r="R67" s="79"/>
+      <c r="R67" s="85"/>
       <c r="S67" s="68">
         <v>4.0000000000000001E-3</v>
       </c>
@@ -11906,7 +11906,7 @@
       </c>
     </row>
     <row r="68" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="C68" s="79"/>
+      <c r="C68" s="85"/>
       <c r="D68" s="68">
         <v>0.3</v>
       </c>
@@ -11918,7 +11918,7 @@
         <f t="shared" si="25"/>
         <v>7.1009800588459114E-3</v>
       </c>
-      <c r="H68" s="79"/>
+      <c r="H68" s="85"/>
       <c r="I68" s="68">
         <v>0.3</v>
       </c>
@@ -11930,7 +11930,7 @@
         <f t="shared" si="27"/>
         <v>8.2882565370303533E-3</v>
       </c>
-      <c r="M68" s="85"/>
+      <c r="M68" s="81"/>
       <c r="N68" s="68">
         <v>0.3</v>
       </c>
@@ -11942,7 +11942,7 @@
         <f t="shared" si="29"/>
         <v>7.5858933457234384E-3</v>
       </c>
-      <c r="R68" s="79"/>
+      <c r="R68" s="85"/>
       <c r="S68" s="68">
         <v>0.3</v>
       </c>
@@ -11956,7 +11956,7 @@
       </c>
     </row>
     <row r="69" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="C69" s="79"/>
+      <c r="C69" s="85"/>
       <c r="D69" s="68">
         <v>5.0000000000000001E-3</v>
       </c>
@@ -11968,7 +11968,7 @@
         <f t="shared" si="25"/>
         <v>1.690799144295819E-4</v>
       </c>
-      <c r="H69" s="79"/>
+      <c r="H69" s="85"/>
       <c r="I69" s="68">
         <v>5.0000000000000001E-3</v>
       </c>
@@ -11980,7 +11980,7 @@
         <f t="shared" si="27"/>
         <v>1.9541011182195101E-4</v>
       </c>
-      <c r="M69" s="85"/>
+      <c r="M69" s="81"/>
       <c r="N69" s="68">
         <v>5.0000000000000001E-3</v>
       </c>
@@ -11992,7 +11992,7 @@
         <f t="shared" si="29"/>
         <v>1.7983382288837E-4</v>
       </c>
-      <c r="R69" s="79"/>
+      <c r="R69" s="85"/>
       <c r="S69" s="68">
         <v>5.0000000000000001E-3</v>
       </c>
@@ -12006,7 +12006,7 @@
       </c>
     </row>
     <row r="70" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="C70" s="79"/>
+      <c r="C70" s="85"/>
       <c r="D70" s="68">
         <v>6.0000000000000001E-3</v>
       </c>
@@ -12018,7 +12018,7 @@
         <f t="shared" si="25"/>
         <v>2.0203459079691096E-4</v>
       </c>
-      <c r="H70" s="79"/>
+      <c r="H70" s="85"/>
       <c r="I70" s="68">
         <v>6.0000000000000001E-3</v>
       </c>
@@ -12030,7 +12030,7 @@
         <f t="shared" si="27"/>
         <v>2.3351975216204669E-4</v>
       </c>
-      <c r="M70" s="86"/>
+      <c r="M70" s="82"/>
       <c r="N70" s="68">
         <v>6.0000000000000001E-3</v>
       </c>
@@ -12042,7 +12042,7 @@
         <f t="shared" si="29"/>
         <v>2.1489391494420996E-4</v>
       </c>
-      <c r="R70" s="79"/>
+      <c r="R70" s="85"/>
       <c r="S70" s="68">
         <v>6.0000000000000001E-3</v>
       </c>
@@ -12082,11 +12082,11 @@
       <c r="F74" s="55" t="s">
         <v>209</v>
       </c>
-      <c r="H74" s="77"/>
-      <c r="I74" s="77"/>
-      <c r="J74" s="77"/>
-      <c r="K74" s="77"/>
-      <c r="L74" s="77"/>
+      <c r="H74" s="87"/>
+      <c r="I74" s="87"/>
+      <c r="J74" s="87"/>
+      <c r="K74" s="87"/>
+      <c r="L74" s="87"/>
     </row>
     <row r="75" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B75" s="55" t="s">
@@ -12107,11 +12107,11 @@
         <f>8.249/(C75*(D75*298.15)^(1/2))</f>
         <v>21.607787805864429</v>
       </c>
-      <c r="H75" s="77"/>
-      <c r="I75" s="77"/>
-      <c r="J75" s="77"/>
-      <c r="K75" s="77"/>
-      <c r="L75" s="77"/>
+      <c r="H75" s="87"/>
+      <c r="I75" s="87"/>
+      <c r="J75" s="87"/>
+      <c r="K75" s="87"/>
+      <c r="L75" s="87"/>
     </row>
     <row r="76" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B76" s="55" t="s">
@@ -12132,11 +12132,11 @@
         <f>8.249/(C76*(D76*298.15)^(1/2))</f>
         <v>2.3435494404947295</v>
       </c>
-      <c r="H76" s="77"/>
-      <c r="I76" s="77"/>
-      <c r="J76" s="77"/>
-      <c r="K76" s="77"/>
-      <c r="L76" s="77"/>
+      <c r="H76" s="87"/>
+      <c r="I76" s="87"/>
+      <c r="J76" s="87"/>
+      <c r="K76" s="87"/>
+      <c r="L76" s="87"/>
     </row>
     <row r="77" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B77" s="55" t="s">
@@ -12157,11 +12157,11 @@
         <f>8.249/(C77*(D77*298.15)^(1/2))</f>
         <v>9.9318548115191021</v>
       </c>
-      <c r="H77" s="77"/>
-      <c r="I77" s="77"/>
-      <c r="J77" s="77"/>
-      <c r="K77" s="77"/>
-      <c r="L77" s="77"/>
+      <c r="H77" s="87"/>
+      <c r="I77" s="87"/>
+      <c r="J77" s="87"/>
+      <c r="K77" s="87"/>
+      <c r="L77" s="87"/>
     </row>
     <row r="78" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B78" s="55" t="s">
@@ -12182,35 +12182,35 @@
         <f>8.249/(C78*(D78*298.15)^(1/2))</f>
         <v>3.5258152609163678</v>
       </c>
-      <c r="H78" s="77"/>
-      <c r="I78" s="77"/>
-      <c r="J78" s="77"/>
-      <c r="K78" s="77"/>
-      <c r="L78" s="77"/>
+      <c r="H78" s="87"/>
+      <c r="I78" s="87"/>
+      <c r="J78" s="87"/>
+      <c r="K78" s="87"/>
+      <c r="L78" s="87"/>
     </row>
     <row r="79" spans="2:21" x14ac:dyDescent="0.25">
       <c r="E79" s="60"/>
-      <c r="H79" s="77"/>
-      <c r="I79" s="77"/>
-      <c r="J79" s="77"/>
-      <c r="K79" s="77"/>
-      <c r="L79" s="77"/>
+      <c r="H79" s="87"/>
+      <c r="I79" s="87"/>
+      <c r="J79" s="87"/>
+      <c r="K79" s="87"/>
+      <c r="L79" s="87"/>
     </row>
     <row r="80" spans="2:21" x14ac:dyDescent="0.25">
       <c r="F80" s="60"/>
-      <c r="H80" s="77"/>
-      <c r="I80" s="77"/>
-      <c r="J80" s="77"/>
-      <c r="K80" s="77"/>
-      <c r="L80" s="77"/>
+      <c r="H80" s="87"/>
+      <c r="I80" s="87"/>
+      <c r="J80" s="87"/>
+      <c r="K80" s="87"/>
+      <c r="L80" s="87"/>
     </row>
     <row r="81" spans="6:12" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F81" s="60"/>
-      <c r="H81" s="77"/>
-      <c r="I81" s="77"/>
-      <c r="J81" s="77"/>
-      <c r="K81" s="77"/>
-      <c r="L81" s="77"/>
+      <c r="H81" s="87"/>
+      <c r="I81" s="87"/>
+      <c r="J81" s="87"/>
+      <c r="K81" s="87"/>
+      <c r="L81" s="87"/>
     </row>
     <row r="82" spans="6:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="F82" s="60"/>
@@ -12232,6 +12232,17 @@
     </row>
   </sheetData>
   <mergeCells count="27">
+    <mergeCell ref="H74:L81"/>
+    <mergeCell ref="H5:K5"/>
+    <mergeCell ref="R46:R57"/>
+    <mergeCell ref="R59:R70"/>
+    <mergeCell ref="R18:U18"/>
+    <mergeCell ref="R20:R31"/>
+    <mergeCell ref="C20:C31"/>
+    <mergeCell ref="H20:H31"/>
+    <mergeCell ref="R33:R44"/>
+    <mergeCell ref="M33:M44"/>
+    <mergeCell ref="M46:M57"/>
     <mergeCell ref="B2:H2"/>
     <mergeCell ref="B1:H1"/>
     <mergeCell ref="B3:H3"/>
@@ -12248,17 +12259,6 @@
     <mergeCell ref="C46:C57"/>
     <mergeCell ref="C59:C70"/>
     <mergeCell ref="H46:H57"/>
-    <mergeCell ref="C20:C31"/>
-    <mergeCell ref="H20:H31"/>
-    <mergeCell ref="R33:R44"/>
-    <mergeCell ref="M33:M44"/>
-    <mergeCell ref="M46:M57"/>
-    <mergeCell ref="H74:L81"/>
-    <mergeCell ref="H5:K5"/>
-    <mergeCell ref="R46:R57"/>
-    <mergeCell ref="R59:R70"/>
-    <mergeCell ref="R18:U18"/>
-    <mergeCell ref="R20:R31"/>
   </mergeCells>
   <conditionalFormatting sqref="C7:F10">
     <cfRule type="colorScale" priority="1">
@@ -12307,20 +12307,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="78" t="s">
+      <c r="A1" s="86" t="s">
         <v>270</v>
       </c>
-      <c r="B1" s="78"/>
-      <c r="C1" s="78"/>
-      <c r="D1" s="78"/>
-      <c r="E1" s="78"/>
-      <c r="G1" s="78" t="s">
+      <c r="B1" s="86"/>
+      <c r="C1" s="86"/>
+      <c r="D1" s="86"/>
+      <c r="E1" s="86"/>
+      <c r="G1" s="86" t="s">
         <v>269</v>
       </c>
-      <c r="H1" s="78"/>
-      <c r="I1" s="78"/>
-      <c r="J1" s="78"/>
-      <c r="L1" s="77" t="s">
+      <c r="H1" s="86"/>
+      <c r="I1" s="86"/>
+      <c r="J1" s="86"/>
+      <c r="L1" s="87" t="s">
         <v>272</v>
       </c>
     </row>
@@ -12348,7 +12348,7 @@
       <c r="J2" s="55" t="s">
         <v>266</v>
       </c>
-      <c r="L2" s="77"/>
+      <c r="L2" s="87"/>
     </row>
     <row r="3" spans="1:25" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A3" s="56" t="s">
@@ -12385,7 +12385,7 @@
         <f>B6/B3</f>
         <v>0.71490423679628545</v>
       </c>
-      <c r="L3" s="77"/>
+      <c r="L3" s="87"/>
     </row>
     <row r="4" spans="1:25" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A4" s="56" t="s">
@@ -12422,7 +12422,7 @@
         <f>C6/C3</f>
         <v>1.175711828778903</v>
       </c>
-      <c r="L4" s="77"/>
+      <c r="L4" s="87"/>
     </row>
     <row r="5" spans="1:25" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A5" s="56" t="s">
@@ -12459,7 +12459,7 @@
         <f>D6/D3</f>
         <v>1.4853163513080128</v>
       </c>
-      <c r="L5" s="77"/>
+      <c r="L5" s="87"/>
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A6" s="56" t="s">
@@ -12496,7 +12496,7 @@
         <f>E6/E3</f>
         <v>0.23742979105818918</v>
       </c>
-      <c r="L6" s="77"/>
+      <c r="L6" s="87"/>
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B7" s="28"/>
@@ -12515,7 +12515,7 @@
         <f>AVERAGE(J3:J6)</f>
         <v>0.90334055198534768</v>
       </c>
-      <c r="L7" s="77"/>
+      <c r="L7" s="87"/>
     </row>
     <row r="8" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B8" s="28"/>
@@ -12535,7 +12535,7 @@
         <f>STDEV(J3:J6)</f>
         <v>0.54523002174006763</v>
       </c>
-      <c r="L8" s="77"/>
+      <c r="L8" s="87"/>
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B9" s="28"/>
@@ -12555,7 +12555,7 @@
         <f>J8/J7</f>
         <v>0.60357084661124716</v>
       </c>
-      <c r="L9" s="77"/>
+      <c r="L9" s="87"/>
     </row>
     <row r="10" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B10" s="28"/>
@@ -12570,30 +12570,30 @@
       <c r="J11" s="71"/>
     </row>
     <row r="12" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="80" t="s">
+      <c r="B12" s="84" t="s">
         <v>228</v>
       </c>
-      <c r="C12" s="80"/>
-      <c r="D12" s="80"/>
-      <c r="E12" s="80"/>
-      <c r="G12" s="80" t="s">
+      <c r="C12" s="84"/>
+      <c r="D12" s="84"/>
+      <c r="E12" s="84"/>
+      <c r="G12" s="84" t="s">
         <v>229</v>
       </c>
-      <c r="H12" s="80"/>
-      <c r="I12" s="80"/>
-      <c r="J12" s="80"/>
-      <c r="L12" s="80" t="s">
+      <c r="H12" s="84"/>
+      <c r="I12" s="84"/>
+      <c r="J12" s="84"/>
+      <c r="L12" s="84" t="s">
         <v>230</v>
       </c>
-      <c r="M12" s="80"/>
-      <c r="N12" s="80"/>
-      <c r="O12" s="80"/>
-      <c r="Q12" s="80" t="s">
+      <c r="M12" s="84"/>
+      <c r="N12" s="84"/>
+      <c r="O12" s="84"/>
+      <c r="Q12" s="84" t="s">
         <v>181</v>
       </c>
-      <c r="R12" s="80"/>
-      <c r="S12" s="80"/>
-      <c r="T12" s="80"/>
+      <c r="R12" s="84"/>
+      <c r="S12" s="84"/>
+      <c r="T12" s="84"/>
     </row>
     <row r="13" spans="1:25" ht="28.5" x14ac:dyDescent="0.25">
       <c r="C13" s="60" t="s">
@@ -12637,7 +12637,7 @@
       </c>
     </row>
     <row r="15" spans="1:25" ht="225" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="84" t="s">
+      <c r="B15" s="80" t="s">
         <v>208</v>
       </c>
       <c r="C15" s="68">
@@ -12651,7 +12651,7 @@
       <c r="E15" s="88" t="s">
         <v>250</v>
       </c>
-      <c r="G15" s="84" t="s">
+      <c r="G15" s="80" t="s">
         <v>208</v>
       </c>
       <c r="H15" s="68">
@@ -12664,7 +12664,7 @@
       <c r="J15" s="68" t="s">
         <v>253</v>
       </c>
-      <c r="L15" s="84" t="s">
+      <c r="L15" s="80" t="s">
         <v>208</v>
       </c>
       <c r="M15" s="68">
@@ -12677,7 +12677,7 @@
       <c r="O15" s="68" t="s">
         <v>252</v>
       </c>
-      <c r="Q15" s="84" t="s">
+      <c r="Q15" s="80" t="s">
         <v>208</v>
       </c>
       <c r="R15" s="68">
@@ -12691,15 +12691,15 @@
       <c r="T15" s="88" t="s">
         <v>262</v>
       </c>
-      <c r="V15" s="87" t="s">
+      <c r="V15" s="83" t="s">
         <v>264</v>
       </c>
-      <c r="W15" s="87"/>
-      <c r="X15" s="87"/>
-      <c r="Y15" s="87"/>
+      <c r="W15" s="83"/>
+      <c r="X15" s="83"/>
+      <c r="Y15" s="83"/>
     </row>
     <row r="16" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="B16" s="85"/>
+      <c r="B16" s="81"/>
       <c r="C16" s="68">
         <f>'[1]House J Org Chem 1971'!B5</f>
         <v>0.5</v>
@@ -12708,8 +12708,8 @@
         <f>'[1]House J Org Chem 1971'!D5</f>
         <v>2.564102564102564E-2</v>
       </c>
-      <c r="E16" s="89"/>
-      <c r="G16" s="85"/>
+      <c r="E16" s="90"/>
+      <c r="G16" s="81"/>
       <c r="H16" s="68">
         <f>'[1]Wypych J Mol Liq 2014'!A7</f>
         <v>1E-3</v>
@@ -12721,7 +12721,7 @@
       <c r="J16" s="88" t="s">
         <v>263</v>
       </c>
-      <c r="L16" s="85"/>
+      <c r="L16" s="81"/>
       <c r="M16" s="68">
         <f>'[1]House J Org Chem 1971'!B9</f>
         <v>1</v>
@@ -12733,7 +12733,7 @@
       <c r="O16" s="88" t="s">
         <v>250</v>
       </c>
-      <c r="Q16" s="85"/>
+      <c r="Q16" s="81"/>
       <c r="R16" s="68">
         <f>'[1]Kalugin Kharkiv Univ Bull 2019 '!C37</f>
         <v>3.4152994999999997E-4</v>
@@ -12742,14 +12742,14 @@
         <f>'[1]Kalugin Kharkiv Univ Bull 2019 '!E37</f>
         <v>5.5266000000000009E-5</v>
       </c>
-      <c r="T16" s="90"/>
-      <c r="V16" s="87"/>
-      <c r="W16" s="87"/>
-      <c r="X16" s="87"/>
-      <c r="Y16" s="87"/>
+      <c r="T16" s="89"/>
+      <c r="V16" s="83"/>
+      <c r="W16" s="83"/>
+      <c r="X16" s="83"/>
+      <c r="Y16" s="83"/>
     </row>
     <row r="17" spans="2:23" ht="127.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="85"/>
+      <c r="B17" s="81"/>
       <c r="C17" s="68">
         <f>'[1]Anand Z Phys Chem 2016'!A6</f>
         <v>5.0310095439384403E-2</v>
@@ -12761,7 +12761,7 @@
       <c r="E17" s="88" t="s">
         <v>260</v>
       </c>
-      <c r="G17" s="85"/>
+      <c r="G17" s="81"/>
       <c r="H17" s="68">
         <f>'[1]Wypych J Mol Liq 2014'!A8</f>
         <v>2E-3</v>
@@ -12770,8 +12770,8 @@
         <f>'[1]Wypych J Mol Liq 2014'!B8</f>
         <v>3.6553980786422442E-4</v>
       </c>
-      <c r="J17" s="90"/>
-      <c r="L17" s="85"/>
+      <c r="J17" s="89"/>
+      <c r="L17" s="81"/>
       <c r="M17" s="68">
         <f>'[1]House J Org Chem 1971'!B10</f>
         <v>0.5</v>
@@ -12780,8 +12780,8 @@
         <f>'[1]House J Org Chem 1971'!D10</f>
         <v>3.0303030303030304E-2</v>
       </c>
-      <c r="O17" s="89"/>
-      <c r="Q17" s="85"/>
+      <c r="O17" s="90"/>
+      <c r="Q17" s="81"/>
       <c r="R17" s="68">
         <f>'[1]Kalugin Kharkiv Univ Bull 2019 '!C38</f>
         <v>3.8171914999999998E-4</v>
@@ -12790,10 +12790,10 @@
         <f>'[1]Kalugin Kharkiv Univ Bull 2019 '!E38</f>
         <v>6.0946000000000002E-5</v>
       </c>
-      <c r="T17" s="90"/>
+      <c r="T17" s="89"/>
     </row>
     <row r="18" spans="2:23" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="85"/>
+      <c r="B18" s="81"/>
       <c r="C18" s="68">
         <f>'[1]Anand Z Phys Chem 2016'!A7</f>
         <v>4.5050031372807997E-2</v>
@@ -12802,8 +12802,8 @@
         <f>'[1]Anand Z Phys Chem 2016'!C7</f>
         <v>6.9661650396890843E-4</v>
       </c>
-      <c r="E18" s="90"/>
-      <c r="G18" s="85"/>
+      <c r="E18" s="89"/>
+      <c r="G18" s="81"/>
       <c r="H18" s="68">
         <f>'[1]Wypych J Mol Liq 2014'!A9</f>
         <v>3.0000000000000001E-3</v>
@@ -12812,8 +12812,8 @@
         <f>'[1]Wypych J Mol Liq 2014'!B9</f>
         <v>5.4341470372513251E-4</v>
       </c>
-      <c r="J18" s="90"/>
-      <c r="L18" s="85"/>
+      <c r="J18" s="89"/>
+      <c r="L18" s="81"/>
       <c r="M18" s="68">
         <f>'[1]Kalugin Kharkiv Univ Bull 2019 '!C12</f>
         <v>7.9658500000000004E-4</v>
@@ -12825,7 +12825,7 @@
       <c r="O18" s="88" t="s">
         <v>262</v>
       </c>
-      <c r="Q18" s="85"/>
+      <c r="Q18" s="81"/>
       <c r="R18" s="68">
         <f>'[1]Kalugin Kharkiv Univ Bull 2019 '!C39</f>
         <v>4.3208084999999996E-4</v>
@@ -12834,10 +12834,10 @@
         <f>'[1]Kalugin Kharkiv Univ Bull 2019 '!E39</f>
         <v>6.8356000000000008E-5</v>
       </c>
-      <c r="T18" s="90"/>
+      <c r="T18" s="89"/>
     </row>
     <row r="19" spans="2:23" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="85"/>
+      <c r="B19" s="81"/>
       <c r="C19" s="68">
         <f>'[1]Anand Z Phys Chem 2016'!A8</f>
         <v>4.0268154948647598E-2</v>
@@ -12846,8 +12846,8 @@
         <f>'[1]Anand Z Phys Chem 2016'!C8</f>
         <v>5.822742283504975E-4</v>
       </c>
-      <c r="E19" s="90"/>
-      <c r="G19" s="85"/>
+      <c r="E19" s="89"/>
+      <c r="G19" s="81"/>
       <c r="H19" s="68">
         <f>'[1]Wypych J Mol Liq 2014'!A10</f>
         <v>4.0000000000000001E-3</v>
@@ -12856,8 +12856,8 @@
         <f>'[1]Wypych J Mol Liq 2014'!B10</f>
         <v>7.190506947066461E-4</v>
       </c>
-      <c r="J19" s="90"/>
-      <c r="L19" s="85"/>
+      <c r="J19" s="89"/>
+      <c r="L19" s="81"/>
       <c r="M19" s="68">
         <f>'[1]Kalugin Kharkiv Univ Bull 2019 '!C13</f>
         <v>9.6583974999999995E-4</v>
@@ -12866,8 +12866,8 @@
         <f>'[1]Kalugin Kharkiv Univ Bull 2019 '!E13</f>
         <v>1.5412000000000002E-4</v>
       </c>
-      <c r="O19" s="90"/>
-      <c r="Q19" s="85"/>
+      <c r="O19" s="89"/>
+      <c r="Q19" s="81"/>
       <c r="R19" s="68">
         <f>'[1]Kalugin Kharkiv Univ Bull 2019 '!C40</f>
         <v>5.8671850000000002E-4</v>
@@ -12876,10 +12876,10 @@
         <f>'[1]Kalugin Kharkiv Univ Bull 2019 '!E40</f>
         <v>9.7729000000000012E-5</v>
       </c>
-      <c r="T19" s="90"/>
+      <c r="T19" s="89"/>
     </row>
     <row r="20" spans="2:23" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="85"/>
+      <c r="B20" s="81"/>
       <c r="C20" s="68">
         <f>'[1]Anand Z Phys Chem 2016'!A9</f>
         <v>3.6203559988111297E-2</v>
@@ -12888,8 +12888,8 @@
         <f>'[1]Anand Z Phys Chem 2016'!C9</f>
         <v>4.6901833621402599E-4</v>
       </c>
-      <c r="E20" s="90"/>
-      <c r="G20" s="85"/>
+      <c r="E20" s="89"/>
+      <c r="G20" s="81"/>
       <c r="H20" s="68">
         <f>'[1]Wypych J Mol Liq 2014'!A11</f>
         <v>5.0000000000000001E-3</v>
@@ -12898,8 +12898,8 @@
         <f>'[1]Wypych J Mol Liq 2014'!B11</f>
         <v>8.9275390098460543E-4</v>
       </c>
-      <c r="J20" s="90"/>
-      <c r="L20" s="85"/>
+      <c r="J20" s="89"/>
+      <c r="L20" s="81"/>
       <c r="M20" s="68">
         <f>'[1]Kalugin Kharkiv Univ Bull 2019 '!C14</f>
         <v>1.3707834999999999E-3</v>
@@ -12908,8 +12908,8 @@
         <f>'[1]Kalugin Kharkiv Univ Bull 2019 '!E14</f>
         <v>2.1596000000000001E-4</v>
       </c>
-      <c r="O20" s="90"/>
-      <c r="Q20" s="85"/>
+      <c r="O20" s="89"/>
+      <c r="Q20" s="81"/>
       <c r="R20" s="68">
         <f>'[1]Kalugin Kharkiv Univ Bull 2019 '!C41</f>
         <v>7.6976089999999996E-4</v>
@@ -12918,10 +12918,10 @@
         <f>'[1]Kalugin Kharkiv Univ Bull 2019 '!E41</f>
         <v>1.1561000000000001E-4</v>
       </c>
-      <c r="T20" s="89"/>
+      <c r="T20" s="90"/>
     </row>
     <row r="21" spans="2:23" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="85"/>
+      <c r="B21" s="81"/>
       <c r="C21" s="68">
         <f>'[1]Anand Z Phys Chem 2016'!A10</f>
         <v>3.0226214457910801E-2</v>
@@ -12930,8 +12930,8 @@
         <f>'[1]Anand Z Phys Chem 2016'!C10</f>
         <v>3.4609465816630875E-4</v>
       </c>
-      <c r="E21" s="90"/>
-      <c r="G21" s="85"/>
+      <c r="E21" s="89"/>
+      <c r="G21" s="81"/>
       <c r="H21" s="68">
         <f>'[1]Wypych J Mol Liq 2014'!A12</f>
         <v>6.0000000000000001E-3</v>
@@ -12940,8 +12940,8 @@
         <f>'[1]Wypych J Mol Liq 2014'!B12</f>
         <v>1.0647308684555239E-3</v>
       </c>
-      <c r="J21" s="90"/>
-      <c r="L21" s="85"/>
+      <c r="J21" s="89"/>
+      <c r="L21" s="81"/>
       <c r="M21" s="68">
         <f>'[1]Kalugin Kharkiv Univ Bull 2019 '!C15</f>
         <v>1.6890262500000002E-3</v>
@@ -12950,8 +12950,8 @@
         <f>'[1]Kalugin Kharkiv Univ Bull 2019 '!E15</f>
         <v>2.6379000000000002E-4</v>
       </c>
-      <c r="O21" s="90"/>
-      <c r="Q21" s="85"/>
+      <c r="O21" s="89"/>
+      <c r="Q21" s="81"/>
       <c r="R21" s="68">
         <f>'[1]Das JCED 1999'!B9</f>
         <v>2.5535000000000002E-3</v>
@@ -12966,7 +12966,7 @@
       <c r="W21" s="60"/>
     </row>
     <row r="22" spans="2:23" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="85"/>
+      <c r="B22" s="81"/>
       <c r="C22" s="68">
         <f>'[1]Anand Z Phys Chem 2016'!A11</f>
         <v>1.99451801459661E-2</v>
@@ -12975,8 +12975,8 @@
         <f>'[1]Anand Z Phys Chem 2016'!C11</f>
         <v>1.6834489332651469E-4</v>
       </c>
-      <c r="E22" s="90"/>
-      <c r="G22" s="85"/>
+      <c r="E22" s="89"/>
+      <c r="G22" s="81"/>
       <c r="H22" s="68">
         <f>'[1]Wypych J Mol Liq 2014'!A13</f>
         <v>7.0000000000000001E-3</v>
@@ -12985,8 +12985,8 @@
         <f>'[1]Wypych J Mol Liq 2014'!B13</f>
         <v>1.2351332277161472E-3</v>
       </c>
-      <c r="J22" s="89"/>
-      <c r="L22" s="85"/>
+      <c r="J22" s="90"/>
+      <c r="L22" s="81"/>
       <c r="M22" s="68">
         <f>'[1]Kalugin Kharkiv Univ Bull 2019 '!C16</f>
         <v>2.04615925E-3</v>
@@ -12995,8 +12995,8 @@
         <f>'[1]Kalugin Kharkiv Univ Bull 2019 '!E16</f>
         <v>3.1684000000000004E-4</v>
       </c>
-      <c r="O22" s="90"/>
-      <c r="Q22" s="85"/>
+      <c r="O22" s="89"/>
+      <c r="Q22" s="81"/>
       <c r="R22" s="68">
         <f>'[1]Das JCED 1999'!B10</f>
         <v>3.5412E-3</v>
@@ -13005,10 +13005,10 @@
         <f>'[1]Das JCED 1999'!D10</f>
         <v>5.7062896799999993E-4</v>
       </c>
-      <c r="T22" s="90"/>
+      <c r="T22" s="89"/>
     </row>
     <row r="23" spans="2:23" ht="142.5" x14ac:dyDescent="0.25">
-      <c r="B23" s="85"/>
+      <c r="B23" s="81"/>
       <c r="C23" s="68">
         <f>'[1]Anand Z Phys Chem 2016'!A12</f>
         <v>1.0142333476437299E-2</v>
@@ -13017,8 +13017,8 @@
         <f>'[1]Anand Z Phys Chem 2016'!C12</f>
         <v>5.5079061725431765E-5</v>
       </c>
-      <c r="E23" s="89"/>
-      <c r="G23" s="85"/>
+      <c r="E23" s="90"/>
+      <c r="G23" s="81"/>
       <c r="H23" s="68">
         <f>'[1]House J Org Chem 1971'!B7</f>
         <v>0.6</v>
@@ -13030,7 +13030,7 @@
       <c r="J23" s="68" t="s">
         <v>250</v>
       </c>
-      <c r="L23" s="85"/>
+      <c r="L23" s="81"/>
       <c r="M23" s="68">
         <f>'[1]Kalugin Kharkiv Univ Bull 2019 '!C17</f>
         <v>2.4298189999999997E-3</v>
@@ -13039,8 +13039,8 @@
         <f>'[1]Kalugin Kharkiv Univ Bull 2019 '!E17</f>
         <v>3.7332000000000006E-4</v>
       </c>
-      <c r="O23" s="90"/>
-      <c r="Q23" s="85"/>
+      <c r="O23" s="89"/>
+      <c r="Q23" s="81"/>
       <c r="R23" s="68">
         <f>'[1]Das JCED 1999'!B11</f>
         <v>4.0008000000000005E-3</v>
@@ -13049,14 +13049,14 @@
         <f>'[1]Das JCED 1999'!D11</f>
         <v>6.3860769600000017E-4</v>
       </c>
-      <c r="T23" s="90"/>
+      <c r="T23" s="89"/>
     </row>
     <row r="24" spans="2:23" ht="64.150000000000006" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="85"/>
+      <c r="B24" s="81"/>
       <c r="C24" s="68"/>
       <c r="D24" s="68"/>
       <c r="E24" s="68"/>
-      <c r="G24" s="85"/>
+      <c r="G24" s="81"/>
       <c r="H24" s="68">
         <f>'[1]Anand Z Phys Chem 2016'!A19</f>
         <v>4.4810937551599997E-2</v>
@@ -13068,7 +13068,7 @@
       <c r="J24" s="88" t="s">
         <v>260</v>
       </c>
-      <c r="L24" s="85"/>
+      <c r="L24" s="81"/>
       <c r="M24" s="68">
         <f>'[1]Anand Z Phys Chem 2016'!A18</f>
         <v>4.9831907796968299E-2</v>
@@ -13077,8 +13077,8 @@
         <f>'[1]Kalugin Kharkiv Univ Bull 2019 '!C18</f>
         <v>2.99541E-3</v>
       </c>
-      <c r="O24" s="89"/>
-      <c r="Q24" s="85"/>
+      <c r="O24" s="90"/>
+      <c r="Q24" s="81"/>
       <c r="R24" s="68">
         <f>'[1]Das JCED 1999'!B12</f>
         <v>4.5163E-3</v>
@@ -13087,14 +13087,14 @@
         <f>'[1]Das JCED 1999'!D12</f>
         <v>7.1362056300000002E-4</v>
       </c>
-      <c r="T24" s="89"/>
+      <c r="T24" s="90"/>
     </row>
     <row r="25" spans="2:23" ht="64.150000000000006" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="85"/>
+      <c r="B25" s="81"/>
       <c r="C25" s="68"/>
       <c r="D25" s="68"/>
       <c r="E25" s="68"/>
-      <c r="G25" s="85"/>
+      <c r="G25" s="81"/>
       <c r="H25" s="68">
         <f>'[1]Anand Z Phys Chem 2016'!A20</f>
         <v>3.6203559988111297E-2</v>
@@ -13103,12 +13103,12 @@
         <f>'[1]Kalugin Kharkiv Univ Bull 2019 '!C20</f>
         <v>0</v>
       </c>
-      <c r="J25" s="90"/>
-      <c r="L25" s="85"/>
+      <c r="J25" s="89"/>
+      <c r="L25" s="81"/>
       <c r="M25" s="68"/>
       <c r="N25" s="68"/>
       <c r="O25" s="68"/>
-      <c r="Q25" s="85"/>
+      <c r="Q25" s="81"/>
       <c r="R25" s="68">
         <f>'[1]Dilo Rev Cub Quim 2010'!A14</f>
         <v>1.0150000000000001E-3</v>
@@ -13122,11 +13122,11 @@
       </c>
     </row>
     <row r="26" spans="2:23" ht="64.150000000000006" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="85"/>
+      <c r="B26" s="81"/>
       <c r="C26" s="68"/>
       <c r="D26" s="68"/>
       <c r="E26" s="68"/>
-      <c r="G26" s="85"/>
+      <c r="G26" s="81"/>
       <c r="H26" s="68">
         <f>'[1]Anand Z Phys Chem 2016'!A21</f>
         <v>4.0029061127439598E-2</v>
@@ -13135,12 +13135,12 @@
         <f>'[1]Kalugin Kharkiv Univ Bull 2019 '!C21</f>
         <v>0</v>
       </c>
-      <c r="J26" s="90"/>
-      <c r="L26" s="85"/>
+      <c r="J26" s="89"/>
+      <c r="L26" s="81"/>
       <c r="M26" s="68"/>
       <c r="N26" s="68"/>
       <c r="O26" s="68"/>
-      <c r="Q26" s="85"/>
+      <c r="Q26" s="81"/>
       <c r="R26" s="68">
         <f>'[1]Dilo Rev Cub Quim 2010'!A15</f>
         <v>2.8806000000000001E-3</v>
@@ -13149,14 +13149,14 @@
         <f>'[1]Dilo Rev Cub Quim 2010'!C15</f>
         <v>4.6530619860000007E-4</v>
       </c>
-      <c r="T26" s="90"/>
+      <c r="T26" s="89"/>
     </row>
     <row r="27" spans="2:23" ht="64.150000000000006" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="85"/>
+      <c r="B27" s="81"/>
       <c r="C27" s="68"/>
       <c r="D27" s="68"/>
       <c r="E27" s="68"/>
-      <c r="G27" s="85"/>
+      <c r="G27" s="81"/>
       <c r="H27" s="68">
         <f>'[1]Anand Z Phys Chem 2016'!A22</f>
         <v>2.9987120636702801E-2</v>
@@ -13165,12 +13165,12 @@
         <f>'[1]Kalugin Kharkiv Univ Bull 2019 '!C22</f>
         <v>0</v>
       </c>
-      <c r="J27" s="90"/>
-      <c r="L27" s="85"/>
+      <c r="J27" s="89"/>
+      <c r="L27" s="81"/>
       <c r="M27" s="68"/>
       <c r="N27" s="68"/>
       <c r="O27" s="68"/>
-      <c r="Q27" s="85"/>
+      <c r="Q27" s="81"/>
       <c r="R27" s="68">
         <f>'[1]Dilo Rev Cub Quim 2010'!A16</f>
         <v>4.6937000000000003E-3</v>
@@ -13179,14 +13179,14 @@
         <f>'[1]Dilo Rev Cub Quim 2010'!C16</f>
         <v>7.3750699990000012E-4</v>
       </c>
-      <c r="T27" s="90"/>
+      <c r="T27" s="89"/>
     </row>
     <row r="28" spans="2:23" ht="64.150000000000006" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="85"/>
+      <c r="B28" s="81"/>
       <c r="C28" s="68"/>
       <c r="D28" s="68"/>
       <c r="E28" s="68"/>
-      <c r="G28" s="85"/>
+      <c r="G28" s="81"/>
       <c r="H28" s="68">
         <f>'[1]Anand Z Phys Chem 2016'!A23</f>
         <v>1.99451801459661E-2</v>
@@ -13195,12 +13195,12 @@
         <f>'[1]Kalugin Kharkiv Univ Bull 2019 '!C23</f>
         <v>0</v>
       </c>
-      <c r="J28" s="89"/>
-      <c r="L28" s="85"/>
+      <c r="J28" s="90"/>
+      <c r="L28" s="81"/>
       <c r="M28" s="68"/>
       <c r="N28" s="68"/>
       <c r="O28" s="68"/>
-      <c r="Q28" s="85"/>
+      <c r="Q28" s="81"/>
       <c r="R28" s="68">
         <f>'[1]Dilo Rev Cub Quim 2010'!A17</f>
         <v>6.5418000000000004E-3</v>
@@ -13209,22 +13209,22 @@
         <f>'[1]Dilo Rev Cub Quim 2010'!C17</f>
         <v>9.7656644580000011E-4</v>
       </c>
-      <c r="T28" s="90"/>
+      <c r="T28" s="89"/>
     </row>
     <row r="29" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="85"/>
+      <c r="B29" s="81"/>
       <c r="C29" s="68"/>
       <c r="D29" s="68"/>
       <c r="E29" s="68"/>
-      <c r="G29" s="85"/>
+      <c r="G29" s="81"/>
       <c r="H29" s="68"/>
       <c r="I29" s="65"/>
       <c r="J29" s="65"/>
-      <c r="L29" s="85"/>
+      <c r="L29" s="81"/>
       <c r="M29" s="68"/>
       <c r="N29" s="68"/>
       <c r="O29" s="68"/>
-      <c r="Q29" s="85"/>
+      <c r="Q29" s="81"/>
       <c r="R29" s="68">
         <f>'[1]Dilo Rev Cub Quim 2010'!A18</f>
         <v>8.4104000000000002E-3</v>
@@ -13233,10 +13233,10 @@
         <f>'[1]Dilo Rev Cub Quim 2010'!C18</f>
         <v>1.2169091864000002E-3</v>
       </c>
-      <c r="T29" s="89"/>
+      <c r="T29" s="90"/>
     </row>
     <row r="30" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B30" s="86"/>
+      <c r="B30" s="82"/>
       <c r="C30" s="72">
         <v>0.3</v>
       </c>
@@ -13247,7 +13247,7 @@
       <c r="E30" s="72" t="s">
         <v>248</v>
       </c>
-      <c r="G30" s="86"/>
+      <c r="G30" s="82"/>
       <c r="H30" s="72">
         <v>0.3</v>
       </c>
@@ -13258,7 +13258,7 @@
       <c r="J30" s="72" t="s">
         <v>248</v>
       </c>
-      <c r="L30" s="86"/>
+      <c r="L30" s="82"/>
       <c r="M30" s="72">
         <v>0.3</v>
       </c>
@@ -13269,7 +13269,7 @@
       <c r="O30" s="72" t="s">
         <v>248</v>
       </c>
-      <c r="Q30" s="86"/>
+      <c r="Q30" s="82"/>
       <c r="R30" s="73">
         <v>0.3</v>
       </c>
@@ -13289,7 +13289,7 @@
       <c r="Q31" s="60"/>
     </row>
     <row r="32" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="84" t="s">
+      <c r="B32" s="80" t="s">
         <v>207</v>
       </c>
       <c r="C32" s="68">
@@ -13303,7 +13303,7 @@
       <c r="E32" s="88" t="s">
         <v>258</v>
       </c>
-      <c r="G32" s="84" t="s">
+      <c r="G32" s="80" t="s">
         <v>207</v>
       </c>
       <c r="H32" s="68">
@@ -13317,7 +13317,7 @@
       <c r="J32" s="88" t="s">
         <v>258</v>
       </c>
-      <c r="L32" s="84" t="s">
+      <c r="L32" s="80" t="s">
         <v>207</v>
       </c>
       <c r="M32" s="68">
@@ -13331,7 +13331,7 @@
       <c r="O32" s="88" t="s">
         <v>251</v>
       </c>
-      <c r="Q32" s="84" t="s">
+      <c r="Q32" s="80" t="s">
         <v>207</v>
       </c>
       <c r="R32" s="68">
@@ -13347,7 +13347,7 @@
       </c>
     </row>
     <row r="33" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="85"/>
+      <c r="B33" s="81"/>
       <c r="C33" s="68">
         <f>'[1]Mukherjee J Phys Chem 1969'!A12</f>
         <v>2E-3</v>
@@ -13356,8 +13356,8 @@
         <f>'[1]Mukherjee J Phys Chem 1969'!B12</f>
         <v>5.3728208474583968E-5</v>
       </c>
-      <c r="E33" s="90"/>
-      <c r="G33" s="85"/>
+      <c r="E33" s="89"/>
+      <c r="G33" s="81"/>
       <c r="H33" s="68">
         <f>'[1]Mukherjee J Phys Chem 1969'!D12</f>
         <v>2E-3</v>
@@ -13366,8 +13366,8 @@
         <f>'[1]Mukherjee J Phys Chem 1969'!E12</f>
         <v>6.2493155818728701E-5</v>
       </c>
-      <c r="J33" s="90"/>
-      <c r="L33" s="85"/>
+      <c r="J33" s="89"/>
+      <c r="L33" s="81"/>
       <c r="M33" s="68">
         <f>'[1]Ue JECS 1994'!A18</f>
         <v>2.77795812819834E-2</v>
@@ -13376,8 +13376,8 @@
         <f>'[1]Ue JECS 1994'!C18</f>
         <v>6.4151492372494E-4</v>
       </c>
-      <c r="O33" s="90"/>
-      <c r="Q33" s="85"/>
+      <c r="O33" s="89"/>
+      <c r="Q33" s="81"/>
       <c r="R33" s="68">
         <f>'[1]Mukherjee J Phys Chem 1969'!H12</f>
         <v>2E-3</v>
@@ -13386,10 +13386,10 @@
         <f>'[1]Mukherjee J Phys Chem 1969'!I12</f>
         <v>6.0609080816895597E-5</v>
       </c>
-      <c r="T33" s="90"/>
+      <c r="T33" s="89"/>
     </row>
     <row r="34" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="85"/>
+      <c r="B34" s="81"/>
       <c r="C34" s="68">
         <f>'[1]Mukherjee J Phys Chem 1969'!A13</f>
         <v>3.0000000000000001E-3</v>
@@ -13398,8 +13398,8 @@
         <f>'[1]Mukherjee J Phys Chem 1969'!B13</f>
         <v>7.9852408146862777E-5</v>
       </c>
-      <c r="E34" s="90"/>
-      <c r="G34" s="85"/>
+      <c r="E34" s="89"/>
+      <c r="G34" s="81"/>
       <c r="H34" s="68">
         <f>'[1]Mukherjee J Phys Chem 1969'!D13</f>
         <v>3.0000000000000001E-3</v>
@@ -13408,8 +13408,8 @@
         <f>'[1]Mukherjee J Phys Chem 1969'!E13</f>
         <v>9.290406228820849E-5</v>
       </c>
-      <c r="J34" s="90"/>
-      <c r="L34" s="85"/>
+      <c r="J34" s="89"/>
+      <c r="L34" s="81"/>
       <c r="M34" s="68">
         <f>'[1]Ue JECS 1994'!A19</f>
         <v>6.06653893688439E-2</v>
@@ -13418,8 +13418,8 @@
         <f>'[1]Ue JECS 1994'!C19</f>
         <v>1.2375235666209502E-3</v>
       </c>
-      <c r="O34" s="90"/>
-      <c r="Q34" s="85"/>
+      <c r="O34" s="89"/>
+      <c r="Q34" s="81"/>
       <c r="R34" s="68">
         <f>'[1]Mukherjee J Phys Chem 1969'!H13</f>
         <v>3.0000000000000001E-3</v>
@@ -13428,10 +13428,10 @@
         <f>'[1]Mukherjee J Phys Chem 1969'!I13</f>
         <v>9.0168179980480397E-5</v>
       </c>
-      <c r="T34" s="90"/>
+      <c r="T34" s="89"/>
     </row>
     <row r="35" spans="2:20" ht="51" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="85"/>
+      <c r="B35" s="81"/>
       <c r="C35" s="68">
         <f>'[1]Mukherjee J Phys Chem 1969'!A14</f>
         <v>4.0000000000000001E-3</v>
@@ -13440,8 +13440,8 @@
         <f>'[1]Mukherjee J Phys Chem 1969'!B14</f>
         <v>1.056922565948685E-4</v>
       </c>
-      <c r="E35" s="89"/>
-      <c r="G35" s="85"/>
+      <c r="E35" s="90"/>
+      <c r="G35" s="81"/>
       <c r="H35" s="68">
         <f>'[1]Mukherjee J Phys Chem 1969'!D14</f>
         <v>4.0000000000000001E-3</v>
@@ -13450,8 +13450,8 @@
         <f>'[1]Mukherjee J Phys Chem 1969'!E14</f>
         <v>1.2297527929804771E-4</v>
       </c>
-      <c r="J35" s="89"/>
-      <c r="L35" s="85"/>
+      <c r="J35" s="90"/>
+      <c r="L35" s="81"/>
       <c r="M35" s="68">
         <f>'[1]Ue JECS 1994'!A20</f>
         <v>8.3327532110991295E-2</v>
@@ -13460,8 +13460,8 @@
         <f>'[1]Ue JECS 1994'!C20</f>
         <v>1.72576387300134E-3</v>
       </c>
-      <c r="O35" s="90"/>
-      <c r="Q35" s="85"/>
+      <c r="O35" s="89"/>
+      <c r="Q35" s="81"/>
       <c r="R35" s="68">
         <f>'[1]Mukherjee J Phys Chem 1969'!H14</f>
         <v>4.0000000000000001E-3</v>
@@ -13470,10 +13470,10 @@
         <f>'[1]Mukherjee J Phys Chem 1969'!I14</f>
         <v>1.194456188645813E-4</v>
       </c>
-      <c r="T35" s="89"/>
+      <c r="T35" s="90"/>
     </row>
     <row r="36" spans="2:20" ht="156.75" x14ac:dyDescent="0.25">
-      <c r="B36" s="85"/>
+      <c r="B36" s="81"/>
       <c r="C36" s="68">
         <f>'[1] Chernozhuk Chem Tech 2016'!A7</f>
         <v>1E-3</v>
@@ -13485,7 +13485,7 @@
       <c r="E36" s="88" t="s">
         <v>257</v>
       </c>
-      <c r="G36" s="85"/>
+      <c r="G36" s="81"/>
       <c r="H36" s="68">
         <v>1</v>
       </c>
@@ -13496,7 +13496,7 @@
       <c r="J36" s="68" t="s">
         <v>251</v>
       </c>
-      <c r="L36" s="85"/>
+      <c r="L36" s="81"/>
       <c r="M36" s="68">
         <f>'[1]Ue JECS 1994'!A21</f>
         <v>0.108230270238364</v>
@@ -13505,8 +13505,8 @@
         <f>'[1]Ue JECS 1994'!C21</f>
         <v>2.2249976506132701E-3</v>
       </c>
-      <c r="O36" s="90"/>
-      <c r="Q36" s="85"/>
+      <c r="O36" s="89"/>
+      <c r="Q36" s="81"/>
       <c r="R36" s="68">
         <f>'[1]Dilo Rev Cub Quim 2010'!A5</f>
         <v>1.0326000000000001E-3</v>
@@ -13520,7 +13520,7 @@
       </c>
     </row>
     <row r="37" spans="2:20" ht="142.5" x14ac:dyDescent="0.25">
-      <c r="B37" s="85"/>
+      <c r="B37" s="81"/>
       <c r="C37" s="68">
         <f>'[1] Chernozhuk Chem Tech 2016'!A8</f>
         <v>2E-3</v>
@@ -13529,8 +13529,8 @@
         <f>'[1] Chernozhuk Chem Tech 2016'!C8</f>
         <v>5.4757247986326682E-5</v>
       </c>
-      <c r="E37" s="90"/>
-      <c r="G37" s="85"/>
+      <c r="E37" s="89"/>
+      <c r="G37" s="81"/>
       <c r="H37" s="68">
         <v>0.65</v>
       </c>
@@ -13540,7 +13540,7 @@
       <c r="J37" s="68" t="s">
         <v>255</v>
       </c>
-      <c r="L37" s="85"/>
+      <c r="L37" s="81"/>
       <c r="M37" s="68">
         <f>'[1]Ue JECS 1994'!A22</f>
         <v>0.13311773213059999</v>
@@ -13549,8 +13549,8 @@
         <f>'[1]Ue JECS 1994'!C22</f>
         <v>2.7016735210060499E-3</v>
       </c>
-      <c r="O37" s="90"/>
-      <c r="Q37" s="85"/>
+      <c r="O37" s="89"/>
+      <c r="Q37" s="81"/>
       <c r="R37" s="68">
         <f>'[1]Dilo Rev Cub Quim 2010'!A6</f>
         <v>2.8214999999999998E-3</v>
@@ -13559,10 +13559,10 @@
         <f>'[1]Dilo Rev Cub Quim 2010'!C6</f>
         <v>8.5098132899999983E-5</v>
       </c>
-      <c r="T37" s="90"/>
+      <c r="T37" s="89"/>
     </row>
     <row r="38" spans="2:20" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="85"/>
+      <c r="B38" s="81"/>
       <c r="C38" s="68">
         <f>'[1] Chernozhuk Chem Tech 2016'!A9</f>
         <v>3.0000000000000001E-3</v>
@@ -13571,12 +13571,12 @@
         <f>'[1] Chernozhuk Chem Tech 2016'!C9</f>
         <v>8.2103807969235025E-5</v>
       </c>
-      <c r="E38" s="89"/>
-      <c r="G38" s="85"/>
+      <c r="E38" s="90"/>
+      <c r="G38" s="81"/>
       <c r="H38" s="68"/>
       <c r="I38" s="68"/>
       <c r="J38" s="68"/>
-      <c r="L38" s="85"/>
+      <c r="L38" s="81"/>
       <c r="M38" s="68">
         <f>'[1]Ue JECS 1994'!A23</f>
         <v>0.160269821037543</v>
@@ -13585,8 +13585,8 @@
         <f>'[1]Ue JECS 1994'!C23</f>
         <v>3.2248295688289802E-3</v>
       </c>
-      <c r="O38" s="90"/>
-      <c r="Q38" s="85"/>
+      <c r="O38" s="89"/>
+      <c r="Q38" s="81"/>
       <c r="R38" s="68">
         <f>'[1]Dilo Rev Cub Quim 2010'!A7</f>
         <v>4.6381E-3</v>
@@ -13595,10 +13595,10 @@
         <f>'[1]Dilo Rev Cub Quim 2010'!C7</f>
         <v>1.3677571376E-4</v>
       </c>
-      <c r="T38" s="90"/>
+      <c r="T38" s="89"/>
     </row>
     <row r="39" spans="2:20" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="85"/>
+      <c r="B39" s="81"/>
       <c r="C39" s="68">
         <f>'[1]Salomon Electr Acta 1983'!B9</f>
         <v>4.9561600000000003E-3</v>
@@ -13610,11 +13610,11 @@
       <c r="E39" s="88" t="s">
         <v>254</v>
       </c>
-      <c r="G39" s="85"/>
+      <c r="G39" s="81"/>
       <c r="H39" s="68"/>
       <c r="I39" s="65"/>
       <c r="J39" s="68"/>
-      <c r="L39" s="85"/>
+      <c r="L39" s="81"/>
       <c r="M39" s="68">
         <v>1</v>
       </c>
@@ -13622,8 +13622,8 @@
         <f>'[1]Ue JECS 1994'!D70</f>
         <v>7.4000000000000003E-3</v>
       </c>
-      <c r="O39" s="89"/>
-      <c r="Q39" s="85"/>
+      <c r="O39" s="90"/>
+      <c r="Q39" s="81"/>
       <c r="R39" s="68">
         <f>'[1]Dilo Rev Cub Quim 2010'!A8</f>
         <v>6.4580000000000002E-3</v>
@@ -13632,10 +13632,10 @@
         <f>'[1]Dilo Rev Cub Quim 2010'!C8</f>
         <v>1.8702367999999999E-4</v>
       </c>
-      <c r="T39" s="90"/>
+      <c r="T39" s="89"/>
     </row>
     <row r="40" spans="2:20" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="85"/>
+      <c r="B40" s="81"/>
       <c r="C40" s="68">
         <f>'[1]Salomon Electr Acta 1983'!B10</f>
         <v>7.5689999999999993E-3</v>
@@ -13644,16 +13644,16 @@
         <f>'[1]Salomon Electr Acta 1983'!D10</f>
         <v>1.5103854135338336E-4</v>
       </c>
-      <c r="E40" s="89"/>
-      <c r="G40" s="85"/>
+      <c r="E40" s="90"/>
+      <c r="G40" s="81"/>
       <c r="H40" s="68"/>
       <c r="I40" s="65"/>
       <c r="J40" s="68"/>
-      <c r="L40" s="85"/>
+      <c r="L40" s="81"/>
       <c r="M40" s="74"/>
       <c r="N40" s="74"/>
       <c r="O40" s="68"/>
-      <c r="Q40" s="85"/>
+      <c r="Q40" s="81"/>
       <c r="R40" s="68">
         <f>'[1]Dilo Rev Cub Quim 2010'!A9</f>
         <v>8.2468999999999997E-3</v>
@@ -13662,10 +13662,10 @@
         <f>'[1]Dilo Rev Cub Quim 2010'!C9</f>
         <v>2.3384827170999997E-4</v>
       </c>
-      <c r="T40" s="89"/>
+      <c r="T40" s="90"/>
     </row>
     <row r="41" spans="2:20" ht="171" x14ac:dyDescent="0.25">
-      <c r="B41" s="85"/>
+      <c r="B41" s="81"/>
       <c r="C41" s="68">
         <v>1</v>
       </c>
@@ -13676,21 +13676,21 @@
       <c r="E41" s="68" t="s">
         <v>251</v>
       </c>
-      <c r="G41" s="85"/>
+      <c r="G41" s="81"/>
       <c r="H41" s="68"/>
       <c r="I41" s="65"/>
       <c r="J41" s="68"/>
-      <c r="L41" s="85"/>
+      <c r="L41" s="81"/>
       <c r="M41" s="74"/>
       <c r="N41" s="74"/>
       <c r="O41" s="68"/>
-      <c r="Q41" s="85"/>
+      <c r="Q41" s="81"/>
       <c r="R41" s="68"/>
       <c r="S41" s="68"/>
       <c r="T41" s="68"/>
     </row>
     <row r="42" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B42" s="86"/>
+      <c r="B42" s="82"/>
       <c r="C42" s="72">
         <v>0.3</v>
       </c>
@@ -13701,7 +13701,7 @@
       <c r="E42" s="72" t="s">
         <v>248</v>
       </c>
-      <c r="G42" s="86"/>
+      <c r="G42" s="82"/>
       <c r="H42" s="72">
         <v>0.3</v>
       </c>
@@ -13712,7 +13712,7 @@
       <c r="J42" s="72" t="s">
         <v>248</v>
       </c>
-      <c r="L42" s="86"/>
+      <c r="L42" s="82"/>
       <c r="M42" s="72">
         <v>0.3</v>
       </c>
@@ -13723,7 +13723,7 @@
       <c r="O42" s="72" t="s">
         <v>248</v>
       </c>
-      <c r="Q42" s="86"/>
+      <c r="Q42" s="82"/>
       <c r="R42" s="73">
         <v>0.3</v>
       </c>
@@ -13736,7 +13736,7 @@
       </c>
     </row>
     <row r="44" spans="2:20" ht="225" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="84" t="s">
+      <c r="B44" s="80" t="s">
         <v>169</v>
       </c>
       <c r="C44" s="68">
@@ -13750,7 +13750,7 @@
       <c r="E44" s="88" t="s">
         <v>250</v>
       </c>
-      <c r="G44" s="84" t="s">
+      <c r="G44" s="80" t="s">
         <v>169</v>
       </c>
       <c r="H44" s="68">
@@ -13763,7 +13763,7 @@
       <c r="J44" s="68" t="s">
         <v>251</v>
       </c>
-      <c r="L44" s="84" t="s">
+      <c r="L44" s="80" t="s">
         <v>169</v>
       </c>
       <c r="M44" s="68">
@@ -13776,7 +13776,7 @@
       <c r="O44" s="68" t="s">
         <v>253</v>
       </c>
-      <c r="Q44" s="84" t="s">
+      <c r="Q44" s="80" t="s">
         <v>169</v>
       </c>
       <c r="R44" s="68">
@@ -13792,7 +13792,7 @@
       </c>
     </row>
     <row r="45" spans="2:20" ht="156.75" x14ac:dyDescent="0.25">
-      <c r="B45" s="85"/>
+      <c r="B45" s="81"/>
       <c r="C45" s="68">
         <f>'[1]House J Org Chem 1971'!B14</f>
         <v>0.5</v>
@@ -13801,8 +13801,8 @@
         <f>'[1]House J Org Chem 1971'!D14</f>
         <v>1.2195121951219513E-2</v>
       </c>
-      <c r="E45" s="89"/>
-      <c r="G45" s="85"/>
+      <c r="E45" s="90"/>
+      <c r="G45" s="81"/>
       <c r="H45" s="68">
         <f>'Debye-Huckel-Onsager'!I51</f>
         <v>1E-3</v>
@@ -13814,7 +13814,7 @@
       <c r="J45" s="88" t="s">
         <v>246</v>
       </c>
-      <c r="L45" s="85"/>
+      <c r="L45" s="81"/>
       <c r="M45" s="68">
         <v>0.1</v>
       </c>
@@ -13825,7 +13825,7 @@
       <c r="O45" s="68" t="s">
         <v>252</v>
       </c>
-      <c r="Q45" s="85"/>
+      <c r="Q45" s="81"/>
       <c r="R45" s="68">
         <f>'[1]Nakata Anal Sci 2001'!H15</f>
         <v>1.7284642569285133E-3</v>
@@ -13834,10 +13834,10 @@
         <f>'[1]Nakata Anal Sci 2001'!J15</f>
         <v>1.4003065501783159E-4</v>
       </c>
-      <c r="T45" s="90"/>
+      <c r="T45" s="89"/>
     </row>
     <row r="46" spans="2:20" ht="156.75" x14ac:dyDescent="0.25">
-      <c r="B46" s="85"/>
+      <c r="B46" s="81"/>
       <c r="C46" s="68">
         <f>'[1]Debye-Huckel-Onsager model'!D55</f>
         <v>1E-3</v>
@@ -13849,7 +13849,7 @@
       <c r="E46" s="68" t="s">
         <v>246</v>
       </c>
-      <c r="G46" s="85"/>
+      <c r="G46" s="81"/>
       <c r="H46" s="68">
         <f>'Debye-Huckel-Onsager'!I52</f>
         <v>2E-3</v>
@@ -13858,8 +13858,8 @@
         <f>'Debye-Huckel-Onsager'!K52</f>
         <v>1.694140502684188E-4</v>
       </c>
-      <c r="J46" s="90"/>
-      <c r="L46" s="85"/>
+      <c r="J46" s="89"/>
+      <c r="L46" s="81"/>
       <c r="M46" s="68">
         <v>1</v>
       </c>
@@ -13870,7 +13870,7 @@
       <c r="O46" s="68" t="s">
         <v>251</v>
       </c>
-      <c r="Q46" s="85"/>
+      <c r="Q46" s="81"/>
       <c r="R46" s="68">
         <f>'[1]Nakata Anal Sci 2001'!H16</f>
         <v>2.6034100068200046E-3</v>
@@ -13879,14 +13879,14 @@
         <f>'[1]Nakata Anal Sci 2001'!J16</f>
         <v>2.0449974256470167E-4</v>
       </c>
-      <c r="T46" s="90"/>
+      <c r="T46" s="89"/>
     </row>
     <row r="47" spans="2:20" ht="142.5" x14ac:dyDescent="0.25">
-      <c r="B47" s="85"/>
+      <c r="B47" s="81"/>
       <c r="C47" s="68"/>
       <c r="D47" s="68"/>
       <c r="E47" s="68"/>
-      <c r="G47" s="85"/>
+      <c r="G47" s="81"/>
       <c r="H47" s="68">
         <f>'Debye-Huckel-Onsager'!I53</f>
         <v>3.0000000000000001E-3</v>
@@ -13895,8 +13895,8 @@
         <f>'Debye-Huckel-Onsager'!K53</f>
         <v>2.519210648029299E-4</v>
       </c>
-      <c r="J47" s="90"/>
-      <c r="L47" s="85"/>
+      <c r="J47" s="89"/>
+      <c r="L47" s="81"/>
       <c r="M47" s="68">
         <f>'[1]House J Org Chem 1971'!B17</f>
         <v>0.5</v>
@@ -13908,7 +13908,7 @@
       <c r="O47" s="68" t="s">
         <v>250</v>
       </c>
-      <c r="Q47" s="85"/>
+      <c r="Q47" s="81"/>
       <c r="R47" s="68">
         <f>'[1]Nakata Anal Sci 2001'!H17</f>
         <v>3.249897699795396E-3</v>
@@ -13917,14 +13917,14 @@
         <f>'[1]Nakata Anal Sci 2001'!J17</f>
         <v>2.4962982331761723E-4</v>
       </c>
-      <c r="T47" s="89"/>
+      <c r="T47" s="90"/>
     </row>
     <row r="48" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B48" s="85"/>
+      <c r="B48" s="81"/>
       <c r="C48" s="68"/>
       <c r="D48" s="68"/>
       <c r="E48" s="68"/>
-      <c r="G48" s="85"/>
+      <c r="G48" s="81"/>
       <c r="H48" s="68">
         <f>'Debye-Huckel-Onsager'!I54</f>
         <v>4.0000000000000001E-3</v>
@@ -13933,12 +13933,12 @@
         <f>'Debye-Huckel-Onsager'!K54</f>
         <v>3.3342182676446568E-4</v>
       </c>
-      <c r="J48" s="90"/>
-      <c r="L48" s="85"/>
+      <c r="J48" s="89"/>
+      <c r="L48" s="81"/>
       <c r="M48" s="68"/>
       <c r="N48" s="68"/>
       <c r="O48" s="68"/>
-      <c r="Q48" s="85"/>
+      <c r="Q48" s="81"/>
       <c r="R48" s="68">
         <f>'[1]Sears JECS 1963'!A5</f>
         <v>8.9660000000000006E-5</v>
@@ -13952,11 +13952,11 @@
       </c>
     </row>
     <row r="49" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B49" s="85"/>
+      <c r="B49" s="81"/>
       <c r="C49" s="68"/>
       <c r="D49" s="68"/>
       <c r="E49" s="68"/>
-      <c r="G49" s="85"/>
+      <c r="G49" s="81"/>
       <c r="H49" s="68">
         <f>'Debye-Huckel-Onsager'!I56</f>
         <v>5.0000000000000001E-3</v>
@@ -13965,12 +13965,12 @@
         <f>'Debye-Huckel-Onsager'!K56</f>
         <v>4.1405391869054877E-4</v>
       </c>
-      <c r="J49" s="90"/>
-      <c r="L49" s="85"/>
+      <c r="J49" s="89"/>
+      <c r="L49" s="81"/>
       <c r="M49" s="68"/>
       <c r="N49" s="68"/>
       <c r="O49" s="68"/>
-      <c r="Q49" s="85"/>
+      <c r="Q49" s="81"/>
       <c r="R49" s="68">
         <f>'[1]Sears JECS 1963'!A6</f>
         <v>2.2450000000000001E-4</v>
@@ -13979,14 +13979,14 @@
         <f>'[1]Sears JECS 1963'!C6</f>
         <v>1.8480839999999997E-5</v>
       </c>
-      <c r="T49" s="90"/>
+      <c r="T49" s="89"/>
     </row>
     <row r="50" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B50" s="85"/>
+      <c r="B50" s="81"/>
       <c r="C50" s="68"/>
       <c r="D50" s="68"/>
       <c r="E50" s="68"/>
-      <c r="G50" s="85"/>
+      <c r="G50" s="81"/>
       <c r="H50" s="68">
         <f>'Debye-Huckel-Onsager'!I57</f>
         <v>6.0000000000000001E-3</v>
@@ -13995,12 +13995,12 @@
         <f>'Debye-Huckel-Onsager'!K57</f>
         <v>4.9391017049178266E-4</v>
       </c>
-      <c r="J50" s="89"/>
-      <c r="L50" s="85"/>
+      <c r="J50" s="90"/>
+      <c r="L50" s="81"/>
       <c r="M50" s="68"/>
       <c r="N50" s="68"/>
       <c r="O50" s="68"/>
-      <c r="Q50" s="85"/>
+      <c r="Q50" s="81"/>
       <c r="R50" s="68">
         <f>'[1]Sears JECS 1963'!A7</f>
         <v>4.1629999999999998E-4</v>
@@ -14009,22 +14009,22 @@
         <f>'[1]Sears JECS 1963'!C7</f>
         <v>3.2679550000000001E-5</v>
       </c>
-      <c r="T50" s="90"/>
+      <c r="T50" s="89"/>
     </row>
     <row r="51" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B51" s="85"/>
+      <c r="B51" s="81"/>
       <c r="C51" s="68"/>
       <c r="D51" s="68"/>
       <c r="E51" s="68"/>
-      <c r="G51" s="85"/>
+      <c r="G51" s="81"/>
       <c r="H51" s="68"/>
       <c r="I51" s="68"/>
       <c r="J51" s="68"/>
-      <c r="L51" s="85"/>
+      <c r="L51" s="81"/>
       <c r="M51" s="68"/>
       <c r="N51" s="68"/>
       <c r="O51" s="68"/>
-      <c r="Q51" s="85"/>
+      <c r="Q51" s="81"/>
       <c r="R51" s="68">
         <f>'[1]Sears JECS 1963'!A8</f>
         <v>6.7409999999999996E-4</v>
@@ -14033,22 +14033,22 @@
         <f>'[1]Sears JECS 1963'!C8</f>
         <v>5.0247414000000001E-5</v>
       </c>
-      <c r="T51" s="90"/>
+      <c r="T51" s="89"/>
     </row>
     <row r="52" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B52" s="85"/>
+      <c r="B52" s="81"/>
       <c r="C52" s="68"/>
       <c r="D52" s="68"/>
       <c r="E52" s="68"/>
-      <c r="G52" s="85"/>
+      <c r="G52" s="81"/>
       <c r="H52" s="68"/>
       <c r="I52" s="65"/>
       <c r="J52" s="65"/>
-      <c r="L52" s="85"/>
+      <c r="L52" s="81"/>
       <c r="M52" s="68"/>
       <c r="N52" s="68"/>
       <c r="O52" s="68"/>
-      <c r="Q52" s="85"/>
+      <c r="Q52" s="81"/>
       <c r="R52" s="68">
         <f>'[1]Sears JECS 1963'!A9</f>
         <v>1.0430000000000001E-3</v>
@@ -14057,22 +14057,22 @@
         <f>'[1]Sears JECS 1963'!C9</f>
         <v>7.3072580000000008E-5</v>
       </c>
-      <c r="T52" s="90"/>
+      <c r="T52" s="89"/>
     </row>
     <row r="53" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B53" s="85"/>
+      <c r="B53" s="81"/>
       <c r="C53" s="68"/>
       <c r="D53" s="68"/>
       <c r="E53" s="68"/>
-      <c r="G53" s="85"/>
+      <c r="G53" s="81"/>
       <c r="H53" s="68"/>
       <c r="I53" s="68"/>
       <c r="J53" s="68"/>
-      <c r="L53" s="85"/>
+      <c r="L53" s="81"/>
       <c r="M53" s="68"/>
       <c r="N53" s="68"/>
       <c r="O53" s="68"/>
-      <c r="Q53" s="85"/>
+      <c r="Q53" s="81"/>
       <c r="R53" s="68">
         <f>'[1]Sears JECS 1963'!A10</f>
         <v>1.629E-3</v>
@@ -14081,10 +14081,10 @@
         <f>'[1]Sears JECS 1963'!C10</f>
         <v>1.0549404000000001E-4</v>
       </c>
-      <c r="T53" s="89"/>
+      <c r="T53" s="90"/>
     </row>
     <row r="54" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B54" s="86"/>
+      <c r="B54" s="82"/>
       <c r="C54" s="72">
         <v>0.3</v>
       </c>
@@ -14095,7 +14095,7 @@
       <c r="E54" s="72" t="s">
         <v>243</v>
       </c>
-      <c r="G54" s="86"/>
+      <c r="G54" s="82"/>
       <c r="H54" s="72">
         <v>0.3</v>
       </c>
@@ -14106,7 +14106,7 @@
       <c r="J54" s="72" t="s">
         <v>248</v>
       </c>
-      <c r="L54" s="86"/>
+      <c r="L54" s="82"/>
       <c r="M54" s="72">
         <v>0.3</v>
       </c>
@@ -14117,7 +14117,7 @@
       <c r="O54" s="72" t="s">
         <v>248</v>
       </c>
-      <c r="Q54" s="86"/>
+      <c r="Q54" s="82"/>
       <c r="R54" s="72">
         <v>0.3</v>
       </c>
@@ -14140,7 +14140,7 @@
       <c r="Q55" s="60"/>
     </row>
     <row r="56" spans="2:20" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B56" s="84" t="s">
+      <c r="B56" s="80" t="s">
         <v>154</v>
       </c>
       <c r="C56" s="68">
@@ -14154,7 +14154,7 @@
       <c r="E56" s="88" t="s">
         <v>247</v>
       </c>
-      <c r="G56" s="84" t="s">
+      <c r="G56" s="80" t="s">
         <v>154</v>
       </c>
       <c r="H56" s="68">
@@ -14168,7 +14168,7 @@
       <c r="J56" s="88" t="s">
         <v>244</v>
       </c>
-      <c r="L56" s="84" t="s">
+      <c r="L56" s="80" t="s">
         <v>154</v>
       </c>
       <c r="M56" s="68">
@@ -14182,7 +14182,7 @@
       <c r="O56" s="88" t="s">
         <v>246</v>
       </c>
-      <c r="Q56" s="84" t="s">
+      <c r="Q56" s="80" t="s">
         <v>154</v>
       </c>
       <c r="R56" s="68">
@@ -14198,7 +14198,7 @@
       </c>
     </row>
     <row r="57" spans="2:20" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B57" s="85"/>
+      <c r="B57" s="81"/>
       <c r="C57" s="68">
         <f>'[1]Butler J Analytical Chem 1966'!A13</f>
         <v>4.0000000000000001E-3</v>
@@ -14207,8 +14207,8 @@
         <f>'[1]Butler J Analytical Chem 1966'!C13</f>
         <v>1.4285582146765418E-4</v>
       </c>
-      <c r="E57" s="90"/>
-      <c r="G57" s="85"/>
+      <c r="E57" s="89"/>
+      <c r="G57" s="81"/>
       <c r="H57" s="68">
         <f>'[1]Anand Z Phys Chem 2019'!B11</f>
         <v>4.3924897114427869E-3</v>
@@ -14217,8 +14217,8 @@
         <f>'[1]Anand Z Phys Chem 2019'!D11</f>
         <v>4.3257238678288523E-4</v>
       </c>
-      <c r="J57" s="90"/>
-      <c r="L57" s="85"/>
+      <c r="J57" s="89"/>
+      <c r="L57" s="81"/>
       <c r="M57" s="68">
         <f>'Debye-Huckel-Onsager'!N65</f>
         <v>2E-3</v>
@@ -14227,8 +14227,8 @@
         <f>'Debye-Huckel-Onsager'!P65</f>
         <v>7.3097347997276484E-5</v>
       </c>
-      <c r="O57" s="90"/>
-      <c r="Q57" s="85"/>
+      <c r="O57" s="89"/>
+      <c r="Q57" s="81"/>
       <c r="R57" s="68">
         <f>'[1]Nakata Anal Sci 2001'!B15</f>
         <v>3.3884176898968934E-3</v>
@@ -14237,10 +14237,10 @@
         <f>'[1]Nakata Anal Sci 2001'!D15</f>
         <v>1.2746020825753812E-4</v>
       </c>
-      <c r="T57" s="90"/>
+      <c r="T57" s="89"/>
     </row>
     <row r="58" spans="2:20" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B58" s="85"/>
+      <c r="B58" s="81"/>
       <c r="C58" s="68">
         <f>'[1]Butler J Analytical Chem 1966'!A14</f>
         <v>5.0000000000000001E-3</v>
@@ -14249,8 +14249,8 @@
         <f>'[1]Butler J Analytical Chem 1966'!C14</f>
         <v>1.7846222104320967E-4</v>
       </c>
-      <c r="E58" s="90"/>
-      <c r="G58" s="85"/>
+      <c r="E58" s="89"/>
+      <c r="G58" s="81"/>
       <c r="H58" s="68">
         <f>'[1]Anand Z Phys Chem 2019'!B12</f>
         <v>4.3924897114427869E-3</v>
@@ -14259,8 +14259,8 @@
         <f>'[1]Anand Z Phys Chem 2019'!D12</f>
         <v>4.3257238678288523E-4</v>
       </c>
-      <c r="J58" s="90"/>
-      <c r="L58" s="85"/>
+      <c r="J58" s="89"/>
+      <c r="L58" s="81"/>
       <c r="M58" s="68">
         <f>'Debye-Huckel-Onsager'!N66</f>
         <v>3.0000000000000001E-3</v>
@@ -14269,8 +14269,8 @@
         <f>'Debye-Huckel-Onsager'!P66</f>
         <v>1.0897089334572343E-4</v>
       </c>
-      <c r="O58" s="90"/>
-      <c r="Q58" s="85"/>
+      <c r="O58" s="89"/>
+      <c r="Q58" s="81"/>
       <c r="R58" s="68">
         <f>'[1]Nakata Anal Sci 2001'!B16</f>
         <v>4.4790988508531544E-3</v>
@@ -14279,10 +14279,10 @@
         <f>'[1]Nakata Anal Sci 2001'!D16</f>
         <v>1.6583833388283441E-4</v>
       </c>
-      <c r="T58" s="90"/>
+      <c r="T58" s="89"/>
     </row>
     <row r="59" spans="2:20" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B59" s="85"/>
+      <c r="B59" s="81"/>
       <c r="C59" s="68">
         <f>'[1]Butler J Analytical Chem 1966'!A15</f>
         <v>6.0000000000000001E-3</v>
@@ -14291,8 +14291,8 @@
         <f>'[1]Butler J Analytical Chem 1966'!C15</f>
         <v>2.1402559830222191E-4</v>
       </c>
-      <c r="E59" s="89"/>
-      <c r="G59" s="85"/>
+      <c r="E59" s="90"/>
+      <c r="G59" s="81"/>
       <c r="H59" s="68">
         <f>'[1]Anand Z Phys Chem 2019'!B13</f>
         <v>4.9506802786069603E-3</v>
@@ -14301,8 +14301,8 @@
         <f>'[1]Anand Z Phys Chem 2019'!D13</f>
         <v>4.8041401423601896E-4</v>
       </c>
-      <c r="J59" s="90"/>
-      <c r="L59" s="85"/>
+      <c r="J59" s="89"/>
+      <c r="L59" s="81"/>
       <c r="M59" s="68">
         <f>'Debye-Huckel-Onsager'!N67</f>
         <v>4.0000000000000001E-3</v>
@@ -14311,8 +14311,8 @@
         <f>'Debye-Huckel-Onsager'!P67</f>
         <v>1.4453564475406955E-4</v>
       </c>
-      <c r="O59" s="89"/>
-      <c r="Q59" s="85"/>
+      <c r="O59" s="90"/>
+      <c r="Q59" s="81"/>
       <c r="R59" s="68">
         <f>'[1]Nakata Anal Sci 2001'!B17</f>
         <v>5.5348968190282854E-3</v>
@@ -14321,10 +14321,10 @@
         <f>'[1]Nakata Anal Sci 2001'!D17</f>
         <v>2.0259805765975052E-4</v>
       </c>
-      <c r="T59" s="89"/>
+      <c r="T59" s="90"/>
     </row>
     <row r="60" spans="2:20" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B60" s="85"/>
+      <c r="B60" s="81"/>
       <c r="C60" s="68">
         <f>'[1]Anand Z Phys Chem 2019'!B23</f>
         <v>3.3040663084577021E-3</v>
@@ -14336,7 +14336,7 @@
       <c r="E60" s="88" t="s">
         <v>244</v>
       </c>
-      <c r="G60" s="85"/>
+      <c r="G60" s="81"/>
       <c r="H60" s="68">
         <f>'[1]Anand Z Phys Chem 2019'!B14</f>
         <v>5.5195923582089515E-3</v>
@@ -14345,18 +14345,18 @@
         <f>'[1]Anand Z Phys Chem 2019'!D14</f>
         <v>5.2414049033552141E-4</v>
       </c>
-      <c r="J60" s="89"/>
-      <c r="L60" s="85"/>
+      <c r="J60" s="90"/>
+      <c r="L60" s="81"/>
       <c r="M60" s="68"/>
       <c r="N60" s="68"/>
       <c r="O60" s="68"/>
-      <c r="Q60" s="85"/>
+      <c r="Q60" s="81"/>
       <c r="R60" s="68"/>
       <c r="S60" s="68"/>
       <c r="T60" s="68"/>
     </row>
     <row r="61" spans="2:20" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B61" s="85"/>
+      <c r="B61" s="81"/>
       <c r="C61" s="68">
         <f>'[1]Anand Z Phys Chem 2019'!B24</f>
         <v>3.9500155223880506E-3</v>
@@ -14365,22 +14365,22 @@
         <f>'[1]Anand Z Phys Chem 2019'!D24</f>
         <v>3.4286134734328236E-4</v>
       </c>
-      <c r="E61" s="90"/>
-      <c r="G61" s="85"/>
+      <c r="E61" s="89"/>
+      <c r="G61" s="81"/>
       <c r="H61" s="68"/>
       <c r="I61" s="65"/>
       <c r="J61" s="65"/>
-      <c r="L61" s="85"/>
+      <c r="L61" s="81"/>
       <c r="M61" s="68"/>
       <c r="N61" s="68"/>
       <c r="O61" s="68"/>
-      <c r="Q61" s="85"/>
+      <c r="Q61" s="81"/>
       <c r="R61" s="68"/>
       <c r="S61" s="68"/>
       <c r="T61" s="68"/>
     </row>
     <row r="62" spans="2:20" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B62" s="85"/>
+      <c r="B62" s="81"/>
       <c r="C62" s="68">
         <f>'[1]Anand Z Phys Chem 2019'!B25</f>
         <v>4.3987122786069638E-3</v>
@@ -14389,22 +14389,22 @@
         <f>'[1]Anand Z Phys Chem 2019'!D25</f>
         <v>3.761778740664671E-4</v>
       </c>
-      <c r="E62" s="90"/>
-      <c r="G62" s="85"/>
+      <c r="E62" s="89"/>
+      <c r="G62" s="81"/>
       <c r="H62" s="68"/>
       <c r="I62" s="65"/>
       <c r="J62" s="65"/>
-      <c r="L62" s="85"/>
+      <c r="L62" s="81"/>
       <c r="M62" s="68"/>
       <c r="N62" s="68"/>
       <c r="O62" s="68"/>
-      <c r="Q62" s="85"/>
+      <c r="Q62" s="81"/>
       <c r="R62" s="68"/>
       <c r="S62" s="68"/>
       <c r="T62" s="68"/>
     </row>
     <row r="63" spans="2:20" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B63" s="85"/>
+      <c r="B63" s="81"/>
       <c r="C63" s="68">
         <f>'[1]Anand Z Phys Chem 2019'!B26</f>
         <v>4.9570781293532262E-3</v>
@@ -14413,22 +14413,22 @@
         <f>'[1]Anand Z Phys Chem 2019'!D26</f>
         <v>4.1917052661810835E-4</v>
       </c>
-      <c r="E63" s="90"/>
-      <c r="G63" s="85"/>
+      <c r="E63" s="89"/>
+      <c r="G63" s="81"/>
       <c r="H63" s="68"/>
       <c r="I63" s="65"/>
       <c r="J63" s="65"/>
-      <c r="L63" s="85"/>
+      <c r="L63" s="81"/>
       <c r="M63" s="68"/>
       <c r="N63" s="68"/>
       <c r="O63" s="68"/>
-      <c r="Q63" s="85"/>
+      <c r="Q63" s="81"/>
       <c r="R63" s="68"/>
       <c r="S63" s="68"/>
       <c r="T63" s="68"/>
     </row>
     <row r="64" spans="2:20" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B64" s="85"/>
+      <c r="B64" s="81"/>
       <c r="C64" s="68">
         <f>'[1]Anand Z Phys Chem 2019'!B27</f>
         <v>5.5151518407960095E-3</v>
@@ -14437,22 +14437,22 @@
         <f>'[1]Anand Z Phys Chem 2019'!D27</f>
         <v>4.5665457241790905E-4</v>
       </c>
-      <c r="E64" s="89"/>
-      <c r="G64" s="85"/>
+      <c r="E64" s="90"/>
+      <c r="G64" s="81"/>
       <c r="H64" s="68"/>
       <c r="I64" s="65"/>
       <c r="J64" s="65"/>
-      <c r="L64" s="85"/>
+      <c r="L64" s="81"/>
       <c r="M64" s="68"/>
       <c r="N64" s="68"/>
       <c r="O64" s="68"/>
-      <c r="Q64" s="85"/>
+      <c r="Q64" s="81"/>
       <c r="R64" s="68"/>
       <c r="S64" s="68"/>
       <c r="T64" s="68"/>
     </row>
     <row r="65" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B65" s="86"/>
+      <c r="B65" s="82"/>
       <c r="C65" s="72">
         <v>0.3</v>
       </c>
@@ -14463,7 +14463,7 @@
       <c r="E65" s="72" t="s">
         <v>243</v>
       </c>
-      <c r="G65" s="86"/>
+      <c r="G65" s="82"/>
       <c r="H65" s="73">
         <v>0.3</v>
       </c>
@@ -14474,7 +14474,7 @@
       <c r="J65" s="73" t="s">
         <v>243</v>
       </c>
-      <c r="L65" s="86"/>
+      <c r="L65" s="82"/>
       <c r="M65" s="73">
         <v>0.3</v>
       </c>
@@ -14485,7 +14485,7 @@
       <c r="O65" s="73" t="s">
         <v>243</v>
       </c>
-      <c r="Q65" s="86"/>
+      <c r="Q65" s="82"/>
       <c r="R65" s="73">
         <v>0.3</v>
       </c>
@@ -14502,20 +14502,25 @@
     </row>
   </sheetData>
   <mergeCells count="49">
-    <mergeCell ref="T44:T47"/>
-    <mergeCell ref="T36:T40"/>
-    <mergeCell ref="T32:T35"/>
-    <mergeCell ref="J32:J35"/>
-    <mergeCell ref="V15:Y16"/>
-    <mergeCell ref="T25:T29"/>
-    <mergeCell ref="T21:T24"/>
-    <mergeCell ref="T15:T20"/>
-    <mergeCell ref="J56:J60"/>
-    <mergeCell ref="E56:E59"/>
-    <mergeCell ref="E60:E64"/>
-    <mergeCell ref="E32:E35"/>
-    <mergeCell ref="E36:E38"/>
-    <mergeCell ref="E39:E40"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="G1:J1"/>
+    <mergeCell ref="B12:E12"/>
+    <mergeCell ref="G12:J12"/>
+    <mergeCell ref="L12:O12"/>
+    <mergeCell ref="L1:L9"/>
+    <mergeCell ref="B44:B54"/>
+    <mergeCell ref="B15:B30"/>
+    <mergeCell ref="Q15:Q30"/>
+    <mergeCell ref="B32:B42"/>
+    <mergeCell ref="G32:G42"/>
+    <mergeCell ref="L32:L42"/>
+    <mergeCell ref="Q32:Q42"/>
+    <mergeCell ref="G15:G30"/>
+    <mergeCell ref="L15:L30"/>
+    <mergeCell ref="E44:E45"/>
+    <mergeCell ref="E15:E16"/>
+    <mergeCell ref="J45:J50"/>
+    <mergeCell ref="E17:E23"/>
     <mergeCell ref="T56:T59"/>
     <mergeCell ref="T48:T53"/>
     <mergeCell ref="Q12:T12"/>
@@ -14532,25 +14537,20 @@
     <mergeCell ref="O16:O17"/>
     <mergeCell ref="O18:O24"/>
     <mergeCell ref="O32:O39"/>
-    <mergeCell ref="B44:B54"/>
-    <mergeCell ref="B15:B30"/>
-    <mergeCell ref="Q15:Q30"/>
-    <mergeCell ref="B32:B42"/>
-    <mergeCell ref="G32:G42"/>
-    <mergeCell ref="L32:L42"/>
-    <mergeCell ref="Q32:Q42"/>
-    <mergeCell ref="G15:G30"/>
-    <mergeCell ref="L15:L30"/>
-    <mergeCell ref="E44:E45"/>
-    <mergeCell ref="E15:E16"/>
-    <mergeCell ref="J45:J50"/>
-    <mergeCell ref="E17:E23"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="G1:J1"/>
-    <mergeCell ref="B12:E12"/>
-    <mergeCell ref="G12:J12"/>
-    <mergeCell ref="L12:O12"/>
-    <mergeCell ref="L1:L9"/>
+    <mergeCell ref="J56:J60"/>
+    <mergeCell ref="E56:E59"/>
+    <mergeCell ref="E60:E64"/>
+    <mergeCell ref="E32:E35"/>
+    <mergeCell ref="E36:E38"/>
+    <mergeCell ref="E39:E40"/>
+    <mergeCell ref="T44:T47"/>
+    <mergeCell ref="T36:T40"/>
+    <mergeCell ref="T32:T35"/>
+    <mergeCell ref="J32:J35"/>
+    <mergeCell ref="V15:Y16"/>
+    <mergeCell ref="T25:T29"/>
+    <mergeCell ref="T21:T24"/>
+    <mergeCell ref="T15:T20"/>
   </mergeCells>
   <conditionalFormatting sqref="B3:E6">
     <cfRule type="colorScale" priority="1">

</xml_diff>